<commit_message>
Moved the Jupyter notebook in a dedicated directory.
</commit_message>
<xml_diff>
--- a/Test Configurations/LHCD/ALOHA_Results.xlsx
+++ b/Test Configurations/LHCD/ALOHA_Results.xlsx
@@ -1728,8 +1728,8 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>323600</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>103415</xdr:rowOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2463,10 +2463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K76"/>
+  <dimension ref="A2:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64:E69"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -3388,7 +3388,9 @@
         <v>90</v>
       </c>
       <c r="E64" s="10"/>
-      <c r="F64" s="7"/>
+      <c r="F64" s="7">
+        <v>13.1028</v>
+      </c>
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
       <c r="I64" s="7"/>
@@ -3401,7 +3403,9 @@
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
       <c r="E65" s="10"/>
-      <c r="F65" s="7"/>
+      <c r="F65" s="7">
+        <v>26.848500000000001</v>
+      </c>
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
@@ -3414,7 +3418,9 @@
       <c r="C66" s="10"/>
       <c r="D66" s="10"/>
       <c r="E66" s="10"/>
-      <c r="F66" s="7"/>
+      <c r="F66" s="7">
+        <v>30.725999999999999</v>
+      </c>
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
       <c r="I66" s="7"/>
@@ -3427,7 +3433,9 @@
       <c r="C67" s="10"/>
       <c r="D67" s="10"/>
       <c r="E67" s="10"/>
-      <c r="F67" s="7"/>
+      <c r="F67" s="7">
+        <v>9.0615000000000006</v>
+      </c>
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
@@ -3440,7 +3448,9 @@
       <c r="C68" s="10"/>
       <c r="D68" s="10"/>
       <c r="E68" s="10"/>
-      <c r="F68" s="7"/>
+      <c r="F68" s="7">
+        <v>2.7608999999999999</v>
+      </c>
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
       <c r="I68" s="7"/>
@@ -3453,7 +3463,9 @@
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
       <c r="E69" s="10"/>
-      <c r="F69" s="7"/>
+      <c r="F69" s="7">
+        <v>19.866399999999999</v>
+      </c>
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
@@ -3473,63 +3485,12 @@
       <c r="J70" s="8"/>
       <c r="K70" s="7"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A71" s="10">
-        <v>2</v>
-      </c>
-      <c r="B71" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="C71" s="10">
-        <v>0</v>
-      </c>
-      <c r="D71" s="10">
-        <v>90</v>
-      </c>
-      <c r="E71" s="10"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A72" s="10"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-      <c r="E72" s="10"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A73" s="10"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
-      <c r="E73" s="10"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A74" s="10"/>
-      <c r="B74" s="10"/>
-      <c r="C74" s="10"/>
-      <c r="D74" s="10"/>
-      <c r="E74" s="10"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A75" s="10"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-      <c r="E75" s="10"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A76" s="10"/>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
-      <c r="E76" s="10"/>
-    </row>
   </sheetData>
-  <mergeCells count="52">
+  <mergeCells count="47">
     <mergeCell ref="D43:D48"/>
     <mergeCell ref="D50:D55"/>
     <mergeCell ref="D27:D32"/>
     <mergeCell ref="E43:E48"/>
-    <mergeCell ref="E71:E76"/>
     <mergeCell ref="D64:D69"/>
     <mergeCell ref="E57:E62"/>
     <mergeCell ref="E50:E55"/>
@@ -3549,9 +3510,6 @@
     <mergeCell ref="A27:A32"/>
     <mergeCell ref="B27:B32"/>
     <mergeCell ref="C27:C32"/>
-    <mergeCell ref="A71:A76"/>
-    <mergeCell ref="B71:B76"/>
-    <mergeCell ref="C71:C76"/>
     <mergeCell ref="J50:J55"/>
     <mergeCell ref="A57:A62"/>
     <mergeCell ref="B57:B62"/>
@@ -3561,7 +3519,6 @@
     <mergeCell ref="B50:B55"/>
     <mergeCell ref="C50:C55"/>
     <mergeCell ref="D57:D62"/>
-    <mergeCell ref="D71:D76"/>
     <mergeCell ref="A64:A69"/>
     <mergeCell ref="B64:B69"/>
     <mergeCell ref="C64:C69"/>

</xml_diff>

<commit_message>
latest results on LH coupling
</commit_message>
<xml_diff>
--- a/Test Configurations/LHCD/ALOHA_Results.xlsx
+++ b/Test Configurations/LHCD/ALOHA_Results.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="6 waveguides" sheetId="1" r:id="rId1"/>
-    <sheet name="12 waveguides" sheetId="4" r:id="rId2"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId3"/>
+    <sheet name="6waveguides_avg" sheetId="2" r:id="rId2"/>
+    <sheet name="12 waveguides" sheetId="4" r:id="rId3"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>HFSS</t>
   </si>
@@ -46,7 +46,28 @@
     <t>Delta Phi [deg]</t>
   </si>
   <si>
-    <t>Number of tetra</t>
+    <t>Number of tetra for 1e-3 convergence target</t>
+  </si>
+  <si>
+    <t>Ne/Nc</t>
+  </si>
+  <si>
+    <t>Avg RC ALOHA</t>
+  </si>
+  <si>
+    <t>Avg RC HFSS</t>
+  </si>
+  <si>
+    <t>Avg RC ALOHA-1</t>
+  </si>
+  <si>
+    <t>Avg RC HFSS-1</t>
+  </si>
+  <si>
+    <t>Ln</t>
+  </si>
+  <si>
+    <t>dgap</t>
   </si>
 </sst>
 </file>
@@ -111,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -147,6 +168,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -186,7 +208,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'6 waveguides'!$F$2</c:f>
+              <c:f>'6 waveguides'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -197,7 +219,7 @@
           </c:tx>
           <c:yVal>
             <c:numRef>
-              <c:f>'6 waveguides'!$F$35:$F$40</c:f>
+              <c:f>'6 waveguides'!$F$34:$F$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -229,7 +251,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'6 waveguides'!$G$2</c:f>
+              <c:f>'6 waveguides'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -240,7 +262,7 @@
           </c:tx>
           <c:yVal>
             <c:numRef>
-              <c:f>'6 waveguides'!$G$35:$G$40</c:f>
+              <c:f>'6 waveguides'!$G$34:$G$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -362,7 +384,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'6 waveguides'!$F$2</c:f>
+              <c:f>'6 waveguides'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -373,7 +395,7 @@
           </c:tx>
           <c:yVal>
             <c:numRef>
-              <c:f>'6 waveguides'!$F$11:$F$16</c:f>
+              <c:f>'6 waveguides'!$F$10:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -405,7 +427,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'6 waveguides'!$G$2</c:f>
+              <c:f>'6 waveguides'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -416,7 +438,7 @@
           </c:tx>
           <c:yVal>
             <c:numRef>
-              <c:f>'6 waveguides'!$G$11:$G$16</c:f>
+              <c:f>'6 waveguides'!$G$10:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -538,7 +560,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'6 waveguides'!$F$2</c:f>
+              <c:f>'6 waveguides'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -549,7 +571,7 @@
           </c:tx>
           <c:yVal>
             <c:numRef>
-              <c:f>'6 waveguides'!$F$50:$F$55</c:f>
+              <c:f>'6 waveguides'!$F$49:$F$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -581,7 +603,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'6 waveguides'!$G$2</c:f>
+              <c:f>'6 waveguides'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -592,7 +614,7 @@
           </c:tx>
           <c:yVal>
             <c:numRef>
-              <c:f>'6 waveguides'!$G$50:$G$55</c:f>
+              <c:f>'6 waveguides'!$G$49:$G$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -627,27 +649,27 @@
           </c:tx>
           <c:yVal>
             <c:numRef>
-              <c:f>'6 waveguides'!$I$57:$I$62</c:f>
+              <c:f>'6 waveguides'!$G$56:$G$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>30.8</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47.8</c:v>
+                  <c:v>32.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.6</c:v>
+                  <c:v>29.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.4</c:v>
+                  <c:v>20.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30</c:v>
+                  <c:v>22.1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>65.599999999999994</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -749,7 +771,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'6 waveguides'!$F$2</c:f>
+              <c:f>'6 waveguides'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -760,7 +782,7 @@
           </c:tx>
           <c:yVal>
             <c:numRef>
-              <c:f>'6 waveguides'!$F$19:$F$24</c:f>
+              <c:f>'6 waveguides'!$F$18:$F$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -792,7 +814,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'6 waveguides'!$G$2</c:f>
+              <c:f>'6 waveguides'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -803,7 +825,7 @@
           </c:tx>
           <c:yVal>
             <c:numRef>
-              <c:f>'6 waveguides'!$G$19:$G$24</c:f>
+              <c:f>'6 waveguides'!$G$18:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -925,7 +947,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'6 waveguides'!$F$2</c:f>
+              <c:f>'6 waveguides'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -936,7 +958,7 @@
           </c:tx>
           <c:yVal>
             <c:numRef>
-              <c:f>'6 waveguides'!$F$27:$F$32</c:f>
+              <c:f>'6 waveguides'!$F$26:$F$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -968,7 +990,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'6 waveguides'!$G$2</c:f>
+              <c:f>'6 waveguides'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -979,7 +1001,7 @@
           </c:tx>
           <c:yVal>
             <c:numRef>
-              <c:f>'6 waveguides'!$G$27:$G$32</c:f>
+              <c:f>'6 waveguides'!$G$26:$G$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1101,7 +1123,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'6 waveguides'!$F$2</c:f>
+              <c:f>'6 waveguides'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1112,7 +1134,7 @@
           </c:tx>
           <c:yVal>
             <c:numRef>
-              <c:f>'6 waveguides'!$F$3:$F$8</c:f>
+              <c:f>'6 waveguides'!$F$2:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1144,7 +1166,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'6 waveguides'!$G$2</c:f>
+              <c:f>'6 waveguides'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1155,7 +1177,7 @@
           </c:tx>
           <c:yVal>
             <c:numRef>
-              <c:f>'6 waveguides'!$G$3:$G$8</c:f>
+              <c:f>'6 waveguides'!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1263,42 +1285,54 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'6 waveguides'!$F$2</c:f>
+              <c:f>'6waveguides_avg'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ALOHA 1D</c:v>
+                  <c:v>Avg RC ALOHA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'6waveguides_avg'!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'6 waveguides'!$F$43:$F$48</c:f>
+              <c:f>'6waveguides_avg'!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.7204000000000002</c:v>
+                  <c:v>13.797716666666666</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.9610000000000003</c:v>
+                  <c:v>23.428250000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.8318999999999992</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.2614999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.1017</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13.913500000000001</c:v>
+                  <c:v>17.061016666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1306,77 +1340,54 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>"ALOHA2D"</c:v>
-          </c:tx>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'6 waveguides'!$H$43:$H$48</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.6583</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.4530000000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.18</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.27600000000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.5004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>21.040199999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="2"/>
-          <c:tx>
             <c:strRef>
-              <c:f>'6 waveguides'!$G$2</c:f>
+              <c:f>'6waveguides_avg'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>HFSS</c:v>
+                  <c:v>Avg RC HFSS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'6waveguides_avg'!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'6 waveguides'!$G$43:$G$48</c:f>
+              <c:f>'6waveguides_avg'!$E$2:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.5</c:v>
+                  <c:v>16.983333333333331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.9</c:v>
+                  <c:v>33.699999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>19.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>51.6</c:v>
+                  <c:v>23.149999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1391,11 +1402,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="218471040"/>
-        <c:axId val="218476928"/>
+        <c:axId val="92192768"/>
+        <c:axId val="49673344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="218471040"/>
+        <c:axId val="92192768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1405,12 +1416,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="218476928"/>
+        <c:crossAx val="49673344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218476928"/>
+        <c:axId val="49673344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1421,7 +1432,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="218471040"/>
+        <c:crossAx val="92192768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1640,6 +1651,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1660,13 +1672,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>2556511</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>21771</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>293914</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>261257</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1690,13 +1702,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>2718705</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>10885</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>108856</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1722,13 +1734,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>2873331</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>21772</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>323600</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1754,7 +1766,7 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>462643</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>54429</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="814197" cy="264560"/>
@@ -1804,9 +1816,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>168729</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>127908</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="814197" cy="264560"/>
@@ -1858,7 +1870,7 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>462643</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>54429</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="814197" cy="264560"/>
@@ -1910,13 +1922,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>2718705</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>266701</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>108856</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>261257</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1942,13 +1954,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>2631619</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>190501</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>21770</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>185058</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1975,12 +1987,12 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>29933</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>97971</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>250371</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2002,22 +2014,27 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>232906</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>82138</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1150620</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>62345</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>49480</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="13" name="Graphique 12"/>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2026,7 +2043,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2035,7 +2052,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2463,10 +2480,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K70"/>
+  <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2476,58 +2494,77 @@
     <col min="6" max="7" width="11.5546875" style="4"/>
     <col min="8" max="9" width="11.44140625" style="4"/>
     <col min="10" max="10" width="42" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="11.44140625" style="3"/>
+    <col min="11" max="22" width="11.44140625" style="3"/>
+    <col min="23" max="23" width="9.6640625" style="3" customWidth="1"/>
+    <col min="24" max="24" width="20.88671875" style="3" customWidth="1"/>
+    <col min="25" max="25" width="19.5546875" style="3" customWidth="1"/>
+    <col min="26" max="26" width="22" style="3" customWidth="1"/>
+    <col min="27" max="27" width="22.33203125" style="3" customWidth="1"/>
+    <col min="28" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="63" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:10" ht="147" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A2" s="10">
+        <v>5</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="C2" s="10">
+        <v>1</v>
+      </c>
+      <c r="D2" s="10">
+        <v>90</v>
+      </c>
+      <c r="E2" s="10">
+        <v>109558</v>
+      </c>
+      <c r="F2" s="4">
+        <v>17.448499999999999</v>
+      </c>
+      <c r="G2" s="4">
+        <v>18.7</v>
+      </c>
+    </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A3" s="10">
-        <v>5</v>
-      </c>
-      <c r="B3" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="C3" s="10">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10">
-        <v>90</v>
-      </c>
-      <c r="E3" s="10">
-        <v>109558</v>
-      </c>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="4">
-        <v>17.448499999999999</v>
+        <v>13.7263</v>
       </c>
       <c r="G3" s="4">
-        <v>18.7</v>
+        <v>17.899999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
@@ -2537,10 +2574,10 @@
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="4">
-        <v>13.7263</v>
+        <v>25.708600000000001</v>
       </c>
       <c r="G4" s="4">
-        <v>17.899999999999999</v>
+        <v>21.8</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
@@ -2550,10 +2587,10 @@
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="4">
-        <v>25.708600000000001</v>
+        <v>14.989800000000001</v>
       </c>
       <c r="G5" s="4">
-        <v>21.8</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
@@ -2563,10 +2600,10 @@
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="4">
-        <v>14.989800000000001</v>
+        <v>3.9382000000000001</v>
       </c>
       <c r="G6" s="4">
-        <v>14.2</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
@@ -2576,65 +2613,68 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="4">
-        <v>3.9382000000000001</v>
+        <v>6.9748999999999999</v>
       </c>
       <c r="G7" s="4">
-        <v>4.3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="4">
-        <v>6.9748999999999999</v>
-      </c>
-      <c r="G8" s="4">
-        <v>25</v>
-      </c>
+      <c r="F8" s="1">
+        <f>AVERAGE(F2:F6)</f>
+        <v>15.162279999999999</v>
+      </c>
+      <c r="G8" s="1">
+        <f>AVERAGE(G2:G6)</f>
+        <v>15.379999999999999</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="F9" s="1">
-        <f>AVERAGE(F3:F8)</f>
-        <v>13.797716666666666</v>
-      </c>
-      <c r="G9" s="1">
-        <f>AVERAGE(G3:G8)</f>
-        <v>16.983333333333331</v>
-      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="A10" s="10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="C10" s="10">
+        <v>2</v>
+      </c>
+      <c r="D10" s="10">
+        <v>90</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="4">
+        <v>22.01</v>
+      </c>
+      <c r="G10" s="4">
+        <v>29.5</v>
+      </c>
+      <c r="H10" s="4">
+        <v>18.7</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A11" s="10">
-        <v>3</v>
-      </c>
-      <c r="B11" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="C11" s="10">
-        <v>2</v>
-      </c>
-      <c r="D11" s="10">
-        <v>90</v>
-      </c>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="4">
-        <v>22.01</v>
+        <v>34.229199999999999</v>
       </c>
       <c r="G11" s="4">
-        <v>29.5</v>
+        <v>34.6</v>
       </c>
       <c r="H11" s="4">
-        <v>18.7</v>
+        <v>28.9</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
@@ -2644,13 +2684,13 @@
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="4">
-        <v>34.229199999999999</v>
+        <v>42.771099999999997</v>
       </c>
       <c r="G12" s="4">
-        <v>34.6</v>
+        <v>42.9</v>
       </c>
       <c r="H12" s="4">
-        <v>28.9</v>
+        <v>27.6</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
@@ -2660,13 +2700,13 @@
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="4">
-        <v>42.771099999999997</v>
+        <v>17.750800000000002</v>
       </c>
       <c r="G13" s="4">
-        <v>42.9</v>
+        <v>18.8</v>
       </c>
       <c r="H13" s="4">
-        <v>27.6</v>
+        <v>16.600000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
@@ -2676,13 +2716,13 @@
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="4">
-        <v>17.750800000000002</v>
+        <v>5.008</v>
       </c>
       <c r="G14" s="4">
-        <v>18.8</v>
+        <v>22.9</v>
       </c>
       <c r="H14" s="4">
-        <v>16.600000000000001</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
@@ -2692,76 +2732,76 @@
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="4">
-        <v>5.008</v>
+        <v>18.8004</v>
       </c>
       <c r="G15" s="4">
-        <v>22.9</v>
+        <v>53.5</v>
       </c>
       <c r="H15" s="4">
-        <v>12.4</v>
+        <v>36.299999999999997</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="4">
-        <v>18.8004</v>
-      </c>
-      <c r="G16" s="4">
-        <v>53.5</v>
-      </c>
-      <c r="H16" s="4">
-        <v>36.299999999999997</v>
-      </c>
+      <c r="F16" s="1">
+        <f>AVERAGE(F10:F14)</f>
+        <v>24.353819999999999</v>
+      </c>
+      <c r="G16" s="1">
+        <f>AVERAGE(G10:G14)</f>
+        <v>29.74</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F17" s="1">
-        <f>AVERAGE(F11:F16)</f>
-        <v>23.428250000000002</v>
-      </c>
-      <c r="G17" s="1">
-        <f>AVERAGE(G11:G16)</f>
-        <v>33.699999999999996</v>
-      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="A18" s="10">
+        <v>3</v>
+      </c>
+      <c r="B18" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="C18" s="10">
+        <v>1</v>
+      </c>
+      <c r="D18" s="10">
+        <v>90</v>
+      </c>
+      <c r="E18" s="10">
+        <v>128000</v>
+      </c>
+      <c r="F18" s="4">
+        <v>12.0671</v>
+      </c>
+      <c r="G18" s="4">
+        <v>10.9</v>
+      </c>
+      <c r="H18" s="4">
+        <v>11.1</v>
+      </c>
+      <c r="I18" s="4">
+        <v>34071</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A19" s="10">
-        <v>3</v>
-      </c>
-      <c r="B19" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="C19" s="10">
-        <v>1</v>
-      </c>
-      <c r="D19" s="10">
-        <v>90</v>
-      </c>
-      <c r="E19" s="10">
-        <v>128000</v>
-      </c>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
       <c r="F19" s="4">
-        <v>12.0671</v>
+        <v>17.912600000000001</v>
       </c>
       <c r="G19" s="4">
-        <v>10.9</v>
+        <v>20.5</v>
       </c>
       <c r="H19" s="4">
-        <v>11.1</v>
-      </c>
-      <c r="I19" s="4">
-        <v>34071</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
@@ -2771,13 +2811,13 @@
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="4">
-        <v>17.912600000000001</v>
+        <v>25.714099999999998</v>
       </c>
       <c r="G20" s="4">
-        <v>20.5</v>
+        <v>19</v>
       </c>
       <c r="H20" s="4">
-        <v>20.5</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
@@ -2787,13 +2827,13 @@
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="4">
-        <v>25.714099999999998</v>
+        <v>10.161799999999999</v>
       </c>
       <c r="G21" s="4">
-        <v>19</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="H21" s="4">
-        <v>19.399999999999999</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
@@ -2803,13 +2843,13 @@
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="4">
-        <v>10.161799999999999</v>
+        <v>1.3297000000000001</v>
       </c>
       <c r="G22" s="4">
-        <v>9.3000000000000007</v>
+        <v>7.3</v>
       </c>
       <c r="H22" s="4">
-        <v>9.5</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
@@ -2819,68 +2859,65 @@
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="4">
-        <v>1.3297000000000001</v>
+        <v>12.5923</v>
       </c>
       <c r="G23" s="4">
-        <v>7.3</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="H23" s="4">
-        <v>7.2</v>
+        <v>32.6</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="4">
-        <v>12.5923</v>
-      </c>
-      <c r="G24" s="4">
-        <v>32.200000000000003</v>
-      </c>
-      <c r="H24" s="4">
-        <v>32.6</v>
-      </c>
+      <c r="F24" s="1">
+        <f>AVERAGE(F18:F22)</f>
+        <v>13.437059999999999</v>
+      </c>
+      <c r="G24" s="1">
+        <f>AVERAGE(G18:G22)</f>
+        <v>13.4</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F25" s="1">
-        <f>AVERAGE(F19:F24)</f>
-        <v>13.296266666666666</v>
-      </c>
-      <c r="G25" s="1">
-        <f>AVERAGE(G19:G24)</f>
-        <v>16.533333333333335</v>
-      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="A26" s="10">
+        <v>3</v>
+      </c>
+      <c r="B26" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="C26" s="10">
+        <v>1</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="4">
+        <v>39.430300000000003</v>
+      </c>
+      <c r="G26" s="4">
+        <v>65.7</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A27" s="10">
-        <v>3</v>
-      </c>
-      <c r="B27" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="C27" s="10">
-        <v>1</v>
-      </c>
-      <c r="D27" s="10">
-        <v>0</v>
-      </c>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="4">
-        <v>39.430300000000003</v>
+        <v>74.356399999999994</v>
       </c>
       <c r="G27" s="4">
-        <v>65.7</v>
+        <v>85.1</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
@@ -2890,10 +2927,10 @@
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="4">
-        <v>74.356399999999994</v>
+        <v>107.6146</v>
       </c>
       <c r="G28" s="4">
-        <v>85.1</v>
+        <v>97.8</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.4">
@@ -2906,7 +2943,7 @@
         <v>107.6146</v>
       </c>
       <c r="G29" s="4">
-        <v>97.8</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
@@ -2916,10 +2953,10 @@
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="4">
-        <v>107.6146</v>
+        <v>74.356399999999994</v>
       </c>
       <c r="G30" s="4">
-        <v>98.1</v>
+        <v>85.4</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
@@ -2929,56 +2966,56 @@
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="4">
-        <v>74.356399999999994</v>
+        <v>39.430300000000003</v>
       </c>
       <c r="G31" s="4">
-        <v>85.4</v>
+        <v>64.900000000000006</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="4">
-        <v>39.430300000000003</v>
-      </c>
-      <c r="G32" s="4">
-        <v>64.900000000000006</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F33" s="1">
-        <f>AVERAGE(F27:F32)</f>
+      <c r="F32" s="1">
+        <f>AVERAGE(F26:F31)</f>
         <v>73.800433333333331</v>
       </c>
-      <c r="G33" s="1">
-        <f>AVERAGE(G27:G32)</f>
+      <c r="G32" s="1">
+        <f>AVERAGE(G26:G31)</f>
         <v>82.833333333333329</v>
       </c>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A34" s="10">
+        <v>3</v>
+      </c>
+      <c r="B34" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="C34" s="10">
+        <v>1</v>
+      </c>
+      <c r="D34" s="10">
+        <v>-90</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="4">
+        <v>12.5923</v>
+      </c>
+      <c r="G34" s="4">
+        <v>48</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A35" s="10">
-        <v>3</v>
-      </c>
-      <c r="B35" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="C35" s="10">
-        <v>1</v>
-      </c>
-      <c r="D35" s="10">
-        <v>-90</v>
-      </c>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="4">
-        <v>12.5923</v>
+        <v>1.3297000000000001</v>
       </c>
       <c r="G35" s="4">
-        <v>48</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.4">
@@ -2988,10 +3025,10 @@
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="4">
-        <v>1.3297000000000001</v>
+        <v>10.161799999999999</v>
       </c>
       <c r="G36" s="4">
-        <v>12</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.4">
@@ -3001,10 +3038,10 @@
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
       <c r="F37" s="4">
-        <v>10.161799999999999</v>
+        <v>25.714099999999998</v>
       </c>
       <c r="G37" s="4">
-        <v>11.7</v>
+        <v>26.6</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.4">
@@ -3014,10 +3051,10 @@
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="4">
-        <v>25.714099999999998</v>
+        <v>17.912600000000001</v>
       </c>
       <c r="G38" s="4">
-        <v>26.6</v>
+        <v>27.6</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.4">
@@ -3027,61 +3064,64 @@
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="4">
-        <v>17.912600000000001</v>
+        <v>12.0671</v>
       </c>
       <c r="G39" s="4">
-        <v>27.6</v>
+        <v>13.9</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="4">
-        <v>12.0671</v>
-      </c>
-      <c r="G40" s="4">
-        <v>13.9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F41" s="1">
-        <f>AVERAGE(F35:F40)</f>
+      <c r="F40" s="1">
+        <f>AVERAGE(F34:F39)</f>
         <v>13.296266666666666</v>
       </c>
-      <c r="G41" s="1">
-        <f>AVERAGE(G35:G40)</f>
+      <c r="G40" s="1">
+        <f>AVERAGE(G34:G39)</f>
         <v>23.3</v>
       </c>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A42" s="10">
+        <v>3</v>
+      </c>
+      <c r="B42" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="C42" s="10">
+        <v>0</v>
+      </c>
+      <c r="D42" s="10">
+        <v>90</v>
+      </c>
+      <c r="E42" s="10">
+        <v>800500</v>
+      </c>
+      <c r="F42" s="4">
+        <v>3.7204000000000002</v>
+      </c>
+      <c r="G42" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="H42" s="9">
+        <v>0.6583</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A43" s="10">
-        <v>3</v>
-      </c>
-      <c r="B43" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="C43" s="10">
-        <v>0</v>
-      </c>
-      <c r="D43" s="10">
-        <v>90</v>
-      </c>
-      <c r="E43" s="10">
-        <v>800500</v>
-      </c>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
       <c r="F43" s="4">
-        <v>3.7204000000000002</v>
+        <v>6.9610000000000003</v>
       </c>
       <c r="G43" s="4">
-        <v>1.5</v>
+        <v>23.9</v>
       </c>
       <c r="H43" s="9">
-        <v>0.6583</v>
+        <v>5.4530000000000003</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.4">
@@ -3091,13 +3131,13 @@
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="4">
-        <v>6.9610000000000003</v>
+        <v>9.8318999999999992</v>
       </c>
       <c r="G44" s="4">
-        <v>23.9</v>
+        <v>17.2</v>
       </c>
       <c r="H44" s="9">
-        <v>5.4530000000000003</v>
+        <v>4.18</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.4">
@@ -3107,13 +3147,13 @@
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="4">
-        <v>9.8318999999999992</v>
+        <v>2.2614999999999998</v>
       </c>
       <c r="G45" s="4">
-        <v>17.2</v>
+        <v>5.6</v>
       </c>
       <c r="H45" s="9">
-        <v>4.18</v>
+        <v>0.27600000000000002</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.4">
@@ -3123,13 +3163,13 @@
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="4">
-        <v>2.2614999999999998</v>
+        <v>0.1017</v>
       </c>
       <c r="G46" s="4">
-        <v>5.6</v>
+        <v>19.7</v>
       </c>
       <c r="H46" s="9">
-        <v>0.27600000000000002</v>
+        <v>1.5004</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.4">
@@ -3139,54 +3179,53 @@
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="4">
-        <v>0.1017</v>
+        <v>13.913500000000001</v>
       </c>
       <c r="G47" s="4">
-        <v>19.7</v>
+        <v>51.6</v>
       </c>
       <c r="H47" s="9">
-        <v>1.5004</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="4">
-        <v>13.913500000000001</v>
-      </c>
-      <c r="G48" s="4">
-        <v>51.6</v>
-      </c>
-      <c r="H48" s="9">
         <v>21.040199999999999</v>
       </c>
     </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A49" s="10">
+        <v>2</v>
+      </c>
+      <c r="B49" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="C49" s="10">
+        <v>2</v>
+      </c>
+      <c r="D49" s="10">
+        <v>90</v>
+      </c>
+      <c r="E49" s="10"/>
+      <c r="F49" s="4">
+        <v>23.551300000000001</v>
+      </c>
+      <c r="G49" s="4">
+        <v>26.8</v>
+      </c>
+      <c r="J49" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K49" s="4"/>
+    </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A50" s="10">
-        <v>2</v>
-      </c>
-      <c r="B50" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="C50" s="10">
-        <v>2</v>
-      </c>
-      <c r="D50" s="10">
-        <v>90</v>
-      </c>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="4">
-        <v>23.551300000000001</v>
+        <v>43.546100000000003</v>
       </c>
       <c r="G50" s="4">
-        <v>26.8</v>
-      </c>
-      <c r="J50" s="11" t="s">
-        <v>7</v>
-      </c>
+        <v>48.6</v>
+      </c>
+      <c r="J50" s="11"/>
       <c r="K50" s="4"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.4">
@@ -3196,10 +3235,10 @@
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="4">
-        <v>43.546100000000003</v>
+        <v>46.9146</v>
       </c>
       <c r="G51" s="4">
-        <v>48.6</v>
+        <v>43.8</v>
       </c>
       <c r="J51" s="11"/>
       <c r="K51" s="4"/>
@@ -3211,11 +3250,13 @@
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="4">
-        <v>46.9146</v>
-      </c>
-      <c r="G52" s="4">
-        <v>43.8</v>
-      </c>
+        <v>16.595700000000001</v>
+      </c>
+      <c r="G52" s="5">
+        <v>30.3</v>
+      </c>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
       <c r="J52" s="11"/>
       <c r="K52" s="4"/>
     </row>
@@ -3226,10 +3267,10 @@
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="4">
-        <v>16.595700000000001</v>
+        <v>7.5068999999999999</v>
       </c>
       <c r="G53" s="5">
-        <v>30.3</v>
+        <v>31.1</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
@@ -3243,56 +3284,62 @@
       <c r="D54" s="10"/>
       <c r="E54" s="10"/>
       <c r="F54" s="4">
-        <v>7.5068999999999999</v>
+        <v>26.793700000000001</v>
       </c>
       <c r="G54" s="5">
-        <v>31.1</v>
+        <v>65.2</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="11"/>
       <c r="K54" s="4"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A55" s="10"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="4">
-        <v>26.793700000000001</v>
-      </c>
-      <c r="G55" s="5">
-        <v>65.2</v>
-      </c>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="4"/>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A56" s="10">
+        <v>2</v>
+      </c>
+      <c r="B56" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="C56" s="10">
+        <v>2</v>
+      </c>
+      <c r="D56" s="10">
+        <v>90</v>
+      </c>
+      <c r="E56" s="10">
+        <v>117325</v>
+      </c>
+      <c r="F56" s="7">
+        <v>23.598400000000002</v>
+      </c>
+      <c r="G56" s="4">
+        <v>20</v>
+      </c>
+      <c r="I56" s="4">
+        <v>30.8</v>
+      </c>
+      <c r="J56" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K56" s="4"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A57" s="10">
-        <v>2</v>
-      </c>
-      <c r="B57" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="C57" s="10">
-        <v>2</v>
-      </c>
-      <c r="D57" s="10">
-        <v>90</v>
-      </c>
+      <c r="A57" s="10"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
       <c r="E57" s="10"/>
-      <c r="F57" s="4">
-        <v>23.551300000000001</v>
+      <c r="F57" s="7">
+        <v>43.762799999999999</v>
+      </c>
+      <c r="G57" s="4">
+        <v>32.700000000000003</v>
       </c>
       <c r="I57" s="4">
-        <v>30.8</v>
-      </c>
-      <c r="J57" s="11" t="s">
-        <v>6</v>
-      </c>
+        <v>47.8</v>
+      </c>
+      <c r="J57" s="11"/>
       <c r="K57" s="4"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.4">
@@ -3301,11 +3348,14 @@
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
       <c r="E58" s="10"/>
-      <c r="F58" s="4">
-        <v>43.546100000000003</v>
+      <c r="F58" s="7">
+        <v>47.040199999999999</v>
+      </c>
+      <c r="G58" s="4">
+        <v>29.7</v>
       </c>
       <c r="I58" s="4">
-        <v>47.8</v>
+        <v>43.6</v>
       </c>
       <c r="J58" s="11"/>
       <c r="K58" s="4"/>
@@ -3316,11 +3366,14 @@
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
       <c r="E59" s="10"/>
-      <c r="F59" s="4">
-        <v>46.9146</v>
+      <c r="F59" s="7">
+        <v>16.622800000000002</v>
+      </c>
+      <c r="G59" s="4">
+        <v>20.7</v>
       </c>
       <c r="I59" s="4">
-        <v>43.6</v>
+        <v>34.4</v>
       </c>
       <c r="J59" s="11"/>
       <c r="K59" s="4"/>
@@ -3331,11 +3384,14 @@
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
       <c r="E60" s="10"/>
-      <c r="F60" s="4">
-        <v>16.595700000000001</v>
+      <c r="F60" s="7">
+        <v>7.5644999999999998</v>
+      </c>
+      <c r="G60" s="4">
+        <v>22.1</v>
       </c>
       <c r="I60" s="4">
-        <v>34.4</v>
+        <v>30</v>
       </c>
       <c r="J60" s="11"/>
       <c r="K60" s="4"/>
@@ -3346,52 +3402,61 @@
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
       <c r="E61" s="10"/>
-      <c r="F61" s="4">
-        <v>7.5068999999999999</v>
+      <c r="F61" s="7">
+        <v>26.966899999999999</v>
+      </c>
+      <c r="G61" s="4">
+        <v>40</v>
       </c>
       <c r="I61" s="4">
-        <v>30</v>
+        <v>65.599999999999994</v>
       </c>
       <c r="J61" s="11"/>
       <c r="K61" s="4"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A62" s="10"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="4">
-        <v>26.793700000000001</v>
-      </c>
-      <c r="I62" s="4">
-        <v>65.599999999999994</v>
-      </c>
-      <c r="J62" s="11"/>
+      <c r="J62" s="6"/>
       <c r="K62" s="4"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="J63" s="6"/>
-      <c r="K63" s="4"/>
+      <c r="A63" s="10">
+        <v>2</v>
+      </c>
+      <c r="B63" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="C63" s="10">
+        <v>1</v>
+      </c>
+      <c r="D63" s="10">
+        <v>90</v>
+      </c>
+      <c r="E63" s="10">
+        <v>12510</v>
+      </c>
+      <c r="F63" s="7">
+        <v>13.1028</v>
+      </c>
+      <c r="G63" s="7">
+        <v>14</v>
+      </c>
+      <c r="H63" s="7"/>
+      <c r="I63" s="7"/>
+      <c r="J63" s="8"/>
+      <c r="K63" s="7"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A64" s="10">
-        <v>2</v>
-      </c>
-      <c r="B64" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="C64" s="10">
-        <v>1</v>
-      </c>
-      <c r="D64" s="10">
-        <v>90</v>
-      </c>
+      <c r="A64" s="10"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
       <c r="E64" s="10"/>
       <c r="F64" s="7">
-        <v>13.1028</v>
-      </c>
-      <c r="G64" s="7"/>
+        <v>26.848500000000001</v>
+      </c>
+      <c r="G64" s="7">
+        <v>27.3</v>
+      </c>
       <c r="H64" s="7"/>
       <c r="I64" s="7"/>
       <c r="J64" s="8"/>
@@ -3404,9 +3469,11 @@
       <c r="D65" s="10"/>
       <c r="E65" s="10"/>
       <c r="F65" s="7">
-        <v>26.848500000000001</v>
-      </c>
-      <c r="G65" s="7"/>
+        <v>30.725999999999999</v>
+      </c>
+      <c r="G65" s="7">
+        <v>23.5</v>
+      </c>
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
       <c r="J65" s="8"/>
@@ -3419,9 +3486,11 @@
       <c r="D66" s="10"/>
       <c r="E66" s="10"/>
       <c r="F66" s="7">
-        <v>30.725999999999999</v>
-      </c>
-      <c r="G66" s="7"/>
+        <v>9.0615000000000006</v>
+      </c>
+      <c r="G66" s="7">
+        <v>15.6</v>
+      </c>
       <c r="H66" s="7"/>
       <c r="I66" s="7"/>
       <c r="J66" s="8"/>
@@ -3434,9 +3503,11 @@
       <c r="D67" s="10"/>
       <c r="E67" s="10"/>
       <c r="F67" s="7">
-        <v>9.0615000000000006</v>
-      </c>
-      <c r="G67" s="7"/>
+        <v>2.7608999999999999</v>
+      </c>
+      <c r="G67" s="7">
+        <v>18.899999999999999</v>
+      </c>
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
       <c r="J67" s="8"/>
@@ -3449,23 +3520,23 @@
       <c r="D68" s="10"/>
       <c r="E68" s="10"/>
       <c r="F68" s="7">
-        <v>2.7608999999999999</v>
-      </c>
-      <c r="G68" s="7"/>
+        <v>19.866399999999999</v>
+      </c>
+      <c r="G68" s="7">
+        <v>39.6</v>
+      </c>
       <c r="H68" s="7"/>
       <c r="I68" s="7"/>
       <c r="J68" s="8"/>
       <c r="K68" s="7"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A69" s="10"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="7">
-        <v>19.866399999999999</v>
-      </c>
+      <c r="A69" s="7"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
@@ -3473,69 +3544,149 @@
       <c r="K69" s="7"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A70" s="7"/>
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
-      <c r="G70" s="7"/>
-      <c r="H70" s="7"/>
-      <c r="I70" s="7"/>
-      <c r="J70" s="8"/>
-      <c r="K70" s="7"/>
+      <c r="A70" s="10">
+        <v>2</v>
+      </c>
+      <c r="B70" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="C70" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D70" s="10">
+        <v>90</v>
+      </c>
+      <c r="E70" s="10">
+        <v>324460</v>
+      </c>
+      <c r="F70" s="7">
+        <v>9.0835000000000008</v>
+      </c>
+      <c r="G70" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A71" s="10"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="7">
+        <v>20.680800000000001</v>
+      </c>
+      <c r="G71" s="4">
+        <v>25.6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A72" s="10"/>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="7">
+        <v>23.258500000000002</v>
+      </c>
+      <c r="G72" s="4">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A73" s="10"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="7">
+        <v>5.9359000000000002</v>
+      </c>
+      <c r="G73" s="4">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A74" s="10"/>
+      <c r="B74" s="10"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="7">
+        <v>1.5745</v>
+      </c>
+      <c r="G74" s="4">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A75" s="10"/>
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="7">
+        <v>18.0078</v>
+      </c>
+      <c r="G75" s="4">
+        <v>38.6</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="47">
-    <mergeCell ref="D43:D48"/>
-    <mergeCell ref="D50:D55"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="E43:E48"/>
-    <mergeCell ref="D64:D69"/>
-    <mergeCell ref="E57:E62"/>
-    <mergeCell ref="E50:E55"/>
-    <mergeCell ref="E64:E69"/>
-    <mergeCell ref="A43:A48"/>
-    <mergeCell ref="B43:B48"/>
-    <mergeCell ref="C43:C48"/>
-    <mergeCell ref="A11:A16"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="C11:C16"/>
-    <mergeCell ref="C35:C40"/>
-    <mergeCell ref="B35:B40"/>
-    <mergeCell ref="A35:A40"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="J50:J55"/>
-    <mergeCell ref="A57:A62"/>
-    <mergeCell ref="B57:B62"/>
-    <mergeCell ref="C57:C62"/>
-    <mergeCell ref="J57:J62"/>
-    <mergeCell ref="A50:A55"/>
-    <mergeCell ref="B50:B55"/>
-    <mergeCell ref="C50:C55"/>
-    <mergeCell ref="D57:D62"/>
-    <mergeCell ref="A64:A69"/>
-    <mergeCell ref="B64:B69"/>
-    <mergeCell ref="C64:C69"/>
-    <mergeCell ref="E11:E16"/>
-    <mergeCell ref="E19:E24"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="E35:E40"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="E3:E8"/>
-    <mergeCell ref="D11:D16"/>
-    <mergeCell ref="D19:D24"/>
-    <mergeCell ref="D35:D40"/>
+  <mergeCells count="52">
+    <mergeCell ref="E70:E75"/>
+    <mergeCell ref="D42:D47"/>
+    <mergeCell ref="D49:D54"/>
+    <mergeCell ref="D26:D31"/>
+    <mergeCell ref="E42:E47"/>
+    <mergeCell ref="D63:D68"/>
+    <mergeCell ref="E56:E61"/>
+    <mergeCell ref="E49:E54"/>
+    <mergeCell ref="E63:E68"/>
+    <mergeCell ref="A42:A47"/>
+    <mergeCell ref="B42:B47"/>
+    <mergeCell ref="C42:C47"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="C34:C39"/>
+    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="A70:A75"/>
+    <mergeCell ref="B70:B75"/>
+    <mergeCell ref="C70:C75"/>
+    <mergeCell ref="J49:J54"/>
+    <mergeCell ref="A56:A61"/>
+    <mergeCell ref="B56:B61"/>
+    <mergeCell ref="C56:C61"/>
+    <mergeCell ref="J56:J61"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="C49:C54"/>
+    <mergeCell ref="D56:D61"/>
+    <mergeCell ref="D70:D75"/>
+    <mergeCell ref="A63:A68"/>
+    <mergeCell ref="B63:B68"/>
+    <mergeCell ref="C63:C68"/>
+    <mergeCell ref="E10:E15"/>
+    <mergeCell ref="E18:E23"/>
+    <mergeCell ref="E26:E31"/>
+    <mergeCell ref="E34:E39"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="E2:E7"/>
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="D34:D39"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C10">
+  <conditionalFormatting sqref="C2:C9">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3547,7 +3698,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A10">
+  <conditionalFormatting sqref="A2:A9">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3559,7 +3710,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B10">
+  <conditionalFormatting sqref="B2:B9">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3571,7 +3722,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C64 C1:C2 C70:C1048576">
+  <conditionalFormatting sqref="C10:C63 C1 C69:C70 C76:C1048576">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -3583,7 +3734,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:A64 A1:A2 A70:A1048576">
+  <conditionalFormatting sqref="A10:A63 A1 A69:A70 A76:A1048576">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -3595,7 +3746,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:B64 B1:B2 B70:B1048576">
+  <conditionalFormatting sqref="B10:B63 B1 B69:B70 B76:B1048576">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -3615,6 +3766,147 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="4" max="6" width="21.21875" customWidth="1"/>
+    <col min="7" max="7" width="22.77734375" customWidth="1"/>
+    <col min="8" max="8" width="21.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <f>'6 waveguides'!A2:A7</f>
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <f>'6 waveguides'!B2:B7</f>
+        <v>0.01</v>
+      </c>
+      <c r="C2">
+        <f>'6 waveguides'!C2:C7</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>AVERAGE('6 waveguides'!F2:F7)</f>
+        <v>13.797716666666666</v>
+      </c>
+      <c r="E2">
+        <f>AVERAGE('6 waveguides'!G2:G7)</f>
+        <v>16.983333333333331</v>
+      </c>
+      <c r="F2">
+        <f>AVERAGE('6 waveguides'!F2:F6)</f>
+        <v>15.162279999999999</v>
+      </c>
+      <c r="G2">
+        <f>AVERAGE('6 waveguides'!G2:G6)</f>
+        <v>15.379999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0.01</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <f>AVERAGE('6 waveguides'!F10:F15)</f>
+        <v>23.428250000000002</v>
+      </c>
+      <c r="E3">
+        <f>AVERAGE('6 waveguides'!G10:G15)</f>
+        <v>33.699999999999996</v>
+      </c>
+      <c r="F3">
+        <f>AVERAGE('6 waveguides'!F10:F14)</f>
+        <v>24.353819999999999</v>
+      </c>
+      <c r="G3">
+        <f>AVERAGE('6 waveguides'!G10:G14)</f>
+        <v>29.74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.01</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <f>AVERAGE('6 waveguides'!F63:F68)</f>
+        <v>17.061016666666667</v>
+      </c>
+      <c r="E4">
+        <f>AVERAGE('6 waveguides'!G63:G68)</f>
+        <v>23.149999999999995</v>
+      </c>
+      <c r="F4">
+        <f>AVERAGE('6 waveguides'!F63:F67)</f>
+        <v>16.499940000000002</v>
+      </c>
+      <c r="G4">
+        <f>AVERAGE('6 waveguides'!G63:G67)</f>
+        <v>19.859999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0.01</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I14"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -3831,18 +4123,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>

</xml_diff>

<commit_message>
Updated files (nothing have changed, a typo eliminated in the file name in the notebook) and the revised version of the paper after reviewer comments.
</commit_message>
<xml_diff>
--- a/Test Configurations/LHCD/ALOHA_Results.xlsx
+++ b/Test Configurations/LHCD/ALOHA_Results.xlsx
@@ -187,6 +187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -196,7 +197,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,11 +330,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="429762048"/>
-        <c:axId val="429763584"/>
+        <c:axId val="269036928"/>
+        <c:axId val="269059200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="429762048"/>
+        <c:axId val="269036928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -344,12 +344,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="429763584"/>
+        <c:crossAx val="269059200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="429763584"/>
+        <c:axId val="269059200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -360,7 +360,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="429762048"/>
+        <c:crossAx val="269036928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -493,7 +493,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'6waveguides_RC_HFSS'!$E$40:$J$40</c:f>
+              <c:f>'6waveguides_RC_HFSS'!$E$43:$J$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -528,11 +528,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="372022656"/>
-        <c:axId val="381382656"/>
+        <c:axId val="291930496"/>
+        <c:axId val="291932416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="372022656"/>
+        <c:axId val="291930496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -570,7 +570,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381382656"/>
+        <c:crossAx val="291932416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -578,7 +578,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="381382656"/>
+        <c:axId val="291932416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -618,7 +618,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="372022656"/>
+        <c:crossAx val="291930496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -753,7 +753,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'6waveguides_RC_HFSS'!$E$31:$J$31</c:f>
+              <c:f>'6waveguides_RC_HFSS'!$E$34:$J$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -788,11 +788,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="381513728"/>
-        <c:axId val="357714176"/>
+        <c:axId val="291961856"/>
+        <c:axId val="291968128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="381513728"/>
+        <c:axId val="291961856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,7 +830,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="357714176"/>
+        <c:crossAx val="291968128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -838,7 +838,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="357714176"/>
+        <c:axId val="291968128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -878,7 +878,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381513728"/>
+        <c:crossAx val="291961856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1440,11 +1440,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="207312768"/>
-        <c:axId val="207321344"/>
+        <c:axId val="292013952"/>
+        <c:axId val="292020608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="207312768"/>
+        <c:axId val="292013952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1467,7 +1467,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1484,12 +1483,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="207321344"/>
+        <c:crossAx val="292020608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="207321344"/>
+        <c:axId val="292020608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1517,7 +1516,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1534,7 +1532,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="207312768"/>
+        <c:crossAx val="292013952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2009,7 +2007,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'6waveguides_RC_HFSS'!$A$19:$A$26</c:f>
+              <c:f>'6waveguides_RC_HFSS'!$A$21:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2042,7 +2040,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'6waveguides_RC_HFSS'!$K$19:$K$26</c:f>
+              <c:f>'6waveguides_RC_HFSS'!$K$21:$K$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2083,11 +2081,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358173696"/>
-        <c:axId val="372228096"/>
+        <c:axId val="291718272"/>
+        <c:axId val="291720576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358173696"/>
+        <c:axId val="291718272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -2110,7 +2108,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2127,12 +2124,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="372228096"/>
+        <c:crossAx val="291720576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="372228096"/>
+        <c:axId val="291720576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2160,7 +2157,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2177,7 +2173,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358173696"/>
+        <c:crossAx val="291718272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2393,11 +2389,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="443674624"/>
-        <c:axId val="443676160"/>
+        <c:axId val="291805440"/>
+        <c:axId val="291807232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="443674624"/>
+        <c:axId val="291805440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2407,12 +2403,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="443676160"/>
+        <c:crossAx val="291807232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="443676160"/>
+        <c:axId val="291807232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2423,13 +2419,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="443674624"/>
+        <c:crossAx val="291805440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2568,11 +2565,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="429780352"/>
-        <c:axId val="429659264"/>
+        <c:axId val="270345728"/>
+        <c:axId val="270347264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="429780352"/>
+        <c:axId val="270345728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2582,12 +2579,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="429659264"/>
+        <c:crossAx val="270347264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="429659264"/>
+        <c:axId val="270347264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2598,7 +2595,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="429780352"/>
+        <c:crossAx val="270345728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2779,11 +2776,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="354875648"/>
-        <c:axId val="376463360"/>
+        <c:axId val="270381440"/>
+        <c:axId val="270382976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="354875648"/>
+        <c:axId val="270381440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2793,12 +2790,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="376463360"/>
+        <c:crossAx val="270382976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="376463360"/>
+        <c:axId val="270382976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2809,7 +2806,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="354875648"/>
+        <c:crossAx val="270381440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2954,11 +2951,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="429678976"/>
-        <c:axId val="429680512"/>
+        <c:axId val="270273152"/>
+        <c:axId val="270279040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="429678976"/>
+        <c:axId val="270273152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2968,12 +2965,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="429680512"/>
+        <c:crossAx val="270279040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="429680512"/>
+        <c:axId val="270279040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2984,7 +2981,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="429678976"/>
+        <c:crossAx val="270273152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3130,11 +3127,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="429697280"/>
-        <c:axId val="429699072"/>
+        <c:axId val="270300288"/>
+        <c:axId val="270301824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="429697280"/>
+        <c:axId val="270300288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3144,12 +3141,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="429699072"/>
+        <c:crossAx val="270301824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="429699072"/>
+        <c:axId val="270301824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3160,7 +3157,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="429697280"/>
+        <c:crossAx val="270300288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3306,11 +3303,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="429736320"/>
-        <c:axId val="429737856"/>
+        <c:axId val="270318592"/>
+        <c:axId val="270471936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="429736320"/>
+        <c:axId val="270318592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3320,12 +3317,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="429737856"/>
+        <c:crossAx val="270471936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="429737856"/>
+        <c:axId val="270471936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3336,7 +3333,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="429736320"/>
+        <c:crossAx val="270318592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3410,7 +3407,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'6waveguides_RC_HFSS'!$A$31:$A$40</c:f>
+              <c:f>'6waveguides_RC_HFSS'!$A$34:$A$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3449,7 +3446,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'6waveguides_RC_HFSS'!$D$31:$D$40</c:f>
+              <c:f>'6waveguides_RC_HFSS'!$D$34:$D$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3496,7 +3493,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'6waveguides_RC_HFSS'!$A$19:$A$26</c:f>
+              <c:f>'6waveguides_RC_HFSS'!$A$21:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3529,7 +3526,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'6waveguides_RC_HFSS'!$D$19:$D$26</c:f>
+              <c:f>'6waveguides_RC_HFSS'!$D$21:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3650,11 +3647,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="443563008"/>
-        <c:axId val="443577088"/>
+        <c:axId val="291560832"/>
+        <c:axId val="291567104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="443563008"/>
+        <c:axId val="291560832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3693,12 +3690,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443577088"/>
+        <c:crossAx val="291567104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="443577088"/>
+        <c:axId val="291567104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3719,7 +3716,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443563008"/>
+        <c:crossAx val="291560832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4160,7 +4157,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'6waveguides_RC_HFSS'!$A$31:$A$40</c:f>
+              <c:f>'6waveguides_RC_HFSS'!$A$34:$A$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4199,7 +4196,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'6waveguides_RC_HFSS'!$K$31:$K$40</c:f>
+              <c:f>'6waveguides_RC_HFSS'!$K$34:$K$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4246,11 +4243,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="443598720"/>
-        <c:axId val="443600256"/>
+        <c:axId val="270493568"/>
+        <c:axId val="291463552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="443598720"/>
+        <c:axId val="270493568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -4290,12 +4287,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443600256"/>
+        <c:crossAx val="291463552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="443600256"/>
+        <c:axId val="291463552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4340,7 +4337,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443598720"/>
+        <c:crossAx val="270493568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4507,7 +4504,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'6waveguides_RC_HFSS'!$E$34:$J$34</c:f>
+              <c:f>'6waveguides_RC_HFSS'!$E$37:$J$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4542,11 +4539,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="372643328"/>
-        <c:axId val="356094720"/>
+        <c:axId val="291509760"/>
+        <c:axId val="291511680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="372643328"/>
+        <c:axId val="291509760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4584,7 +4581,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="356094720"/>
+        <c:crossAx val="291511680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4592,7 +4589,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="356094720"/>
+        <c:axId val="291511680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4632,7 +4629,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="372643328"/>
+        <c:crossAx val="291509760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5019,7 +5016,7 @@
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>535865</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>55417</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5045,13 +5042,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>690282</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>65954</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>568312</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>166254</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5075,13 +5072,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1012373</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>89064</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>706582</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>166255</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5105,13 +5102,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>943099</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>109233</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>415636</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5135,13 +5132,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>692728</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>84369</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>831273</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>166255</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5165,13 +5162,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>193964</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>166255</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>110836</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5220,13 +5217,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>96982</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>166255</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1011877</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>138546</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5275,13 +5272,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>409203</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>69273</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>41564</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5330,13 +5327,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>96981</xdr:colOff>
-      <xdr:row>144</xdr:row>
+      <xdr:row>147</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>44284</xdr:colOff>
-      <xdr:row>187</xdr:row>
+      <xdr:row>190</xdr:row>
       <xdr:rowOff>72591</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5362,13 +5359,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>-1</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>99</xdr:row>
       <xdr:rowOff>41563</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>737011</xdr:colOff>
-      <xdr:row>138</xdr:row>
+      <xdr:row>141</xdr:row>
       <xdr:rowOff>141863</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5873,19 +5870,19 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A2" s="11">
+      <c r="A2" s="12">
         <v>5</v>
       </c>
-      <c r="B2" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="C2" s="11">
+      <c r="B2" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="C2" s="12">
         <v>1</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="12">
         <v>90</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="12">
         <v>109558</v>
       </c>
       <c r="F2" s="4">
@@ -5896,11 +5893,11 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
       <c r="F3" s="4">
         <v>13.7263</v>
       </c>
@@ -5909,11 +5906,11 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
       <c r="F4" s="4">
         <v>25.708600000000001</v>
       </c>
@@ -5922,11 +5919,11 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
       <c r="F5" s="4">
         <v>14.989800000000001</v>
       </c>
@@ -5935,11 +5932,11 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
       <c r="F6" s="4">
         <v>3.9382000000000001</v>
       </c>
@@ -5948,11 +5945,11 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
       <c r="F7" s="4">
         <v>6.9748999999999999</v>
       </c>
@@ -5979,19 +5976,19 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A10" s="11">
+      <c r="A10" s="12">
         <v>3</v>
       </c>
-      <c r="B10" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="C10" s="11">
-        <v>2</v>
-      </c>
-      <c r="D10" s="11">
+      <c r="B10" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="C10" s="12">
+        <v>2</v>
+      </c>
+      <c r="D10" s="12">
         <v>90</v>
       </c>
-      <c r="E10" s="11"/>
+      <c r="E10" s="12"/>
       <c r="F10" s="4">
         <v>22.01</v>
       </c>
@@ -6003,11 +6000,11 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="4">
         <v>34.229199999999999</v>
       </c>
@@ -6019,11 +6016,11 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
       <c r="F12" s="4">
         <v>42.771099999999997</v>
       </c>
@@ -6035,11 +6032,11 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
       <c r="F13" s="4">
         <v>17.750800000000002</v>
       </c>
@@ -6051,11 +6048,11 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
       <c r="F14" s="4">
         <v>5.008</v>
       </c>
@@ -6067,11 +6064,11 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
       <c r="F15" s="4">
         <v>18.8004</v>
       </c>
@@ -6101,19 +6098,19 @@
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A18" s="11">
+      <c r="A18" s="12">
         <v>3</v>
       </c>
-      <c r="B18" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="C18" s="11">
+      <c r="B18" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="C18" s="12">
         <v>1</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="12">
         <v>90</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="12">
         <v>128000</v>
       </c>
       <c r="F18" s="4">
@@ -6130,11 +6127,11 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
       <c r="F19" s="4">
         <v>17.912600000000001</v>
       </c>
@@ -6146,11 +6143,11 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
       <c r="F20" s="4">
         <v>25.714099999999998</v>
       </c>
@@ -6162,11 +6159,11 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
       <c r="F21" s="4">
         <v>10.161799999999999</v>
       </c>
@@ -6178,11 +6175,11 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
       <c r="F22" s="4">
         <v>1.3297000000000001</v>
       </c>
@@ -6194,11 +6191,11 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
       <c r="F23" s="4">
         <v>12.5923</v>
       </c>
@@ -6228,19 +6225,19 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A26" s="11">
+      <c r="A26" s="12">
         <v>3</v>
       </c>
-      <c r="B26" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="C26" s="11">
+      <c r="B26" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="C26" s="12">
         <v>1</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="12">
         <v>0</v>
       </c>
-      <c r="E26" s="11"/>
+      <c r="E26" s="12"/>
       <c r="F26" s="4">
         <v>39.430300000000003</v>
       </c>
@@ -6249,11 +6246,11 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
       <c r="F27" s="4">
         <v>74.356399999999994</v>
       </c>
@@ -6262,11 +6259,11 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
       <c r="F28" s="4">
         <v>107.6146</v>
       </c>
@@ -6275,11 +6272,11 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
       <c r="F29" s="4">
         <v>107.6146</v>
       </c>
@@ -6288,11 +6285,11 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
       <c r="F30" s="4">
         <v>74.356399999999994</v>
       </c>
@@ -6301,11 +6298,11 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
       <c r="F31" s="4">
         <v>39.430300000000003</v>
       </c>
@@ -6326,19 +6323,19 @@
       <c r="I32" s="1"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A34" s="11">
+      <c r="A34" s="12">
         <v>3</v>
       </c>
-      <c r="B34" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="C34" s="11">
+      <c r="B34" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="C34" s="12">
         <v>1</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="12">
         <v>-90</v>
       </c>
-      <c r="E34" s="11"/>
+      <c r="E34" s="12"/>
       <c r="F34" s="4">
         <v>12.5923</v>
       </c>
@@ -6347,11 +6344,11 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
       <c r="F35" s="4">
         <v>1.3297000000000001</v>
       </c>
@@ -6360,11 +6357,11 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
       <c r="F36" s="4">
         <v>10.161799999999999</v>
       </c>
@@ -6373,11 +6370,11 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
       <c r="F37" s="4">
         <v>25.714099999999998</v>
       </c>
@@ -6386,11 +6383,11 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
       <c r="F38" s="4">
         <v>17.912600000000001</v>
       </c>
@@ -6399,11 +6396,11 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
       <c r="F39" s="4">
         <v>12.0671</v>
       </c>
@@ -6424,19 +6421,19 @@
       <c r="I40" s="1"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A42" s="11">
+      <c r="A42" s="12">
         <v>3</v>
       </c>
-      <c r="B42" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="C42" s="11">
+      <c r="B42" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="C42" s="12">
         <v>0</v>
       </c>
-      <c r="D42" s="11">
+      <c r="D42" s="12">
         <v>90</v>
       </c>
-      <c r="E42" s="11">
+      <c r="E42" s="12">
         <v>800500</v>
       </c>
       <c r="F42" s="4">
@@ -6450,11 +6447,11 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
       <c r="F43" s="4">
         <v>6.9610000000000003</v>
       </c>
@@ -6466,11 +6463,11 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
       <c r="F44" s="4">
         <v>9.8318999999999992</v>
       </c>
@@ -6482,11 +6479,11 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A45" s="11"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
       <c r="F45" s="4">
         <v>2.2614999999999998</v>
       </c>
@@ -6498,11 +6495,11 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A46" s="11"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
       <c r="F46" s="4">
         <v>0.1017</v>
       </c>
@@ -6514,11 +6511,11 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
       <c r="F47" s="4">
         <v>13.913500000000001</v>
       </c>
@@ -6530,66 +6527,66 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A49" s="11">
-        <v>2</v>
-      </c>
-      <c r="B49" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="C49" s="11">
-        <v>2</v>
-      </c>
-      <c r="D49" s="11">
+      <c r="A49" s="12">
+        <v>2</v>
+      </c>
+      <c r="B49" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="C49" s="12">
+        <v>2</v>
+      </c>
+      <c r="D49" s="12">
         <v>90</v>
       </c>
-      <c r="E49" s="11"/>
+      <c r="E49" s="12"/>
       <c r="F49" s="4">
         <v>23.551300000000001</v>
       </c>
       <c r="G49" s="4">
         <v>26.8</v>
       </c>
-      <c r="J49" s="12" t="s">
+      <c r="J49" s="13" t="s">
         <v>7</v>
       </c>
       <c r="K49" s="4"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A50" s="11"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
       <c r="F50" s="4">
         <v>43.546100000000003</v>
       </c>
       <c r="G50" s="4">
         <v>48.6</v>
       </c>
-      <c r="J50" s="12"/>
+      <c r="J50" s="13"/>
       <c r="K50" s="4"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A51" s="11"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
       <c r="F51" s="4">
         <v>46.9146</v>
       </c>
       <c r="G51" s="4">
         <v>43.8</v>
       </c>
-      <c r="J51" s="12"/>
+      <c r="J51" s="13"/>
       <c r="K51" s="4"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A52" s="11"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
       <c r="F52" s="4">
         <v>16.595700000000001</v>
       </c>
@@ -6598,15 +6595,15 @@
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
-      <c r="J52" s="12"/>
+      <c r="J52" s="13"/>
       <c r="K52" s="4"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A53" s="11"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
       <c r="F53" s="4">
         <v>7.5068999999999999</v>
       </c>
@@ -6615,15 +6612,15 @@
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
-      <c r="J53" s="12"/>
+      <c r="J53" s="13"/>
       <c r="K53" s="4"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A54" s="11"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
       <c r="F54" s="4">
         <v>26.793700000000001</v>
       </c>
@@ -6632,23 +6629,23 @@
       </c>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
-      <c r="J54" s="12"/>
+      <c r="J54" s="13"/>
       <c r="K54" s="4"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A56" s="11">
-        <v>2</v>
-      </c>
-      <c r="B56" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="C56" s="11">
-        <v>2</v>
-      </c>
-      <c r="D56" s="11">
+      <c r="A56" s="12">
+        <v>2</v>
+      </c>
+      <c r="B56" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="C56" s="12">
+        <v>2</v>
+      </c>
+      <c r="D56" s="12">
         <v>90</v>
       </c>
-      <c r="E56" s="11">
+      <c r="E56" s="12">
         <v>117325</v>
       </c>
       <c r="F56" s="7">
@@ -6660,17 +6657,17 @@
       <c r="I56" s="4">
         <v>30.8</v>
       </c>
-      <c r="J56" s="12" t="s">
+      <c r="J56" s="13" t="s">
         <v>6</v>
       </c>
       <c r="K56" s="4"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A57" s="11"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
+      <c r="A57" s="12"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
       <c r="F57" s="7">
         <v>43.762799999999999</v>
       </c>
@@ -6680,15 +6677,15 @@
       <c r="I57" s="4">
         <v>47.8</v>
       </c>
-      <c r="J57" s="12"/>
+      <c r="J57" s="13"/>
       <c r="K57" s="4"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A58" s="11"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
+      <c r="A58" s="12"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
       <c r="F58" s="7">
         <v>47.040199999999999</v>
       </c>
@@ -6698,15 +6695,15 @@
       <c r="I58" s="4">
         <v>43.6</v>
       </c>
-      <c r="J58" s="12"/>
+      <c r="J58" s="13"/>
       <c r="K58" s="4"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A59" s="11"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
+      <c r="A59" s="12"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
       <c r="F59" s="7">
         <v>16.622800000000002</v>
       </c>
@@ -6716,15 +6713,15 @@
       <c r="I59" s="4">
         <v>34.4</v>
       </c>
-      <c r="J59" s="12"/>
+      <c r="J59" s="13"/>
       <c r="K59" s="4"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A60" s="11"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
+      <c r="A60" s="12"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
       <c r="F60" s="7">
         <v>7.5644999999999998</v>
       </c>
@@ -6734,15 +6731,15 @@
       <c r="I60" s="4">
         <v>30</v>
       </c>
-      <c r="J60" s="12"/>
+      <c r="J60" s="13"/>
       <c r="K60" s="4"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A61" s="11"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
       <c r="F61" s="7">
         <v>26.966899999999999</v>
       </c>
@@ -6752,7 +6749,7 @@
       <c r="I61" s="4">
         <v>65.599999999999994</v>
       </c>
-      <c r="J61" s="12"/>
+      <c r="J61" s="13"/>
       <c r="K61" s="4"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.4">
@@ -6760,19 +6757,19 @@
       <c r="K62" s="4"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A63" s="11">
-        <v>2</v>
-      </c>
-      <c r="B63" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="C63" s="11">
+      <c r="A63" s="12">
+        <v>2</v>
+      </c>
+      <c r="B63" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="C63" s="12">
         <v>1</v>
       </c>
-      <c r="D63" s="11">
+      <c r="D63" s="12">
         <v>90</v>
       </c>
-      <c r="E63" s="11">
+      <c r="E63" s="12">
         <v>12510</v>
       </c>
       <c r="F63" s="7">
@@ -6787,11 +6784,11 @@
       <c r="K63" s="7"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A64" s="11"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
+      <c r="A64" s="12"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
       <c r="F64" s="7">
         <v>26.848500000000001</v>
       </c>
@@ -6804,11 +6801,11 @@
       <c r="K64" s="7"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A65" s="11"/>
-      <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
+      <c r="A65" s="12"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
       <c r="F65" s="7">
         <v>30.725999999999999</v>
       </c>
@@ -6821,11 +6818,11 @@
       <c r="K65" s="7"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A66" s="11"/>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
+      <c r="A66" s="12"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
       <c r="F66" s="7">
         <v>9.0615000000000006</v>
       </c>
@@ -6838,11 +6835,11 @@
       <c r="K66" s="7"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A67" s="11"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
+      <c r="A67" s="12"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
       <c r="F67" s="7">
         <v>2.7608999999999999</v>
       </c>
@@ -6855,11 +6852,11 @@
       <c r="K67" s="7"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A68" s="11"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
+      <c r="A68" s="12"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
       <c r="F68" s="7">
         <v>19.866399999999999</v>
       </c>
@@ -6885,19 +6882,19 @@
       <c r="K69" s="7"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A70" s="11">
-        <v>2</v>
-      </c>
-      <c r="B70" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="C70" s="11">
+      <c r="A70" s="12">
+        <v>2</v>
+      </c>
+      <c r="B70" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="C70" s="12">
         <v>0.5</v>
       </c>
-      <c r="D70" s="11">
+      <c r="D70" s="12">
         <v>90</v>
       </c>
-      <c r="E70" s="11">
+      <c r="E70" s="12">
         <v>324460</v>
       </c>
       <c r="F70" s="7">
@@ -6908,11 +6905,11 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A71" s="11"/>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
+      <c r="A71" s="12"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
       <c r="F71" s="7">
         <v>20.680800000000001</v>
       </c>
@@ -6921,11 +6918,11 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A72" s="11"/>
-      <c r="B72" s="11"/>
-      <c r="C72" s="11"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="11"/>
+      <c r="A72" s="12"/>
+      <c r="B72" s="12"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
       <c r="F72" s="7">
         <v>23.258500000000002</v>
       </c>
@@ -6934,11 +6931,11 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A73" s="11"/>
-      <c r="B73" s="11"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
+      <c r="A73" s="12"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
       <c r="F73" s="7">
         <v>5.9359000000000002</v>
       </c>
@@ -6947,11 +6944,11 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A74" s="11"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
+      <c r="A74" s="12"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
       <c r="F74" s="7">
         <v>1.5745</v>
       </c>
@@ -6960,11 +6957,11 @@
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A75" s="11"/>
-      <c r="B75" s="11"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
+      <c r="A75" s="12"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
       <c r="F75" s="7">
         <v>18.0078</v>
       </c>
@@ -6974,30 +6971,18 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="E70:E75"/>
-    <mergeCell ref="D42:D47"/>
-    <mergeCell ref="D49:D54"/>
-    <mergeCell ref="D26:D31"/>
-    <mergeCell ref="E42:E47"/>
-    <mergeCell ref="D63:D68"/>
-    <mergeCell ref="E56:E61"/>
-    <mergeCell ref="E49:E54"/>
-    <mergeCell ref="E63:E68"/>
-    <mergeCell ref="A42:A47"/>
-    <mergeCell ref="B42:B47"/>
-    <mergeCell ref="C42:C47"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="C10:C15"/>
-    <mergeCell ref="C34:C39"/>
-    <mergeCell ref="B34:B39"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="B26:B31"/>
-    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="E10:E15"/>
+    <mergeCell ref="E18:E23"/>
+    <mergeCell ref="E26:E31"/>
+    <mergeCell ref="E34:E39"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="E2:E7"/>
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="D34:D39"/>
     <mergeCell ref="A70:A75"/>
     <mergeCell ref="B70:B75"/>
     <mergeCell ref="C70:C75"/>
@@ -7014,18 +6999,30 @@
     <mergeCell ref="A63:A68"/>
     <mergeCell ref="B63:B68"/>
     <mergeCell ref="C63:C68"/>
-    <mergeCell ref="E10:E15"/>
-    <mergeCell ref="E18:E23"/>
-    <mergeCell ref="E26:E31"/>
-    <mergeCell ref="E34:E39"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="D2:D7"/>
-    <mergeCell ref="E2:E7"/>
-    <mergeCell ref="D10:D15"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="D34:D39"/>
+    <mergeCell ref="A42:A47"/>
+    <mergeCell ref="B42:B47"/>
+    <mergeCell ref="C42:C47"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="C34:C39"/>
+    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="E70:E75"/>
+    <mergeCell ref="D42:D47"/>
+    <mergeCell ref="D49:D54"/>
+    <mergeCell ref="D26:D31"/>
+    <mergeCell ref="E42:E47"/>
+    <mergeCell ref="D63:D68"/>
+    <mergeCell ref="E56:E61"/>
+    <mergeCell ref="E49:E54"/>
+    <mergeCell ref="E63:E68"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C9">
     <cfRule type="colorScale" priority="6">
@@ -7112,7 +7109,7 @@
   </sheetPr>
   <dimension ref="A1:K261"/>
   <sheetViews>
-    <sheetView topLeftCell="A233" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J211" sqref="J211"/>
     </sheetView>
   </sheetViews>
@@ -12821,7 +12818,7 @@
       <c r="A161">
         <v>0.1</v>
       </c>
-      <c r="B161" s="14">
+      <c r="B161" s="11">
         <v>1E-3</v>
       </c>
       <c r="C161">
@@ -12854,7 +12851,7 @@
       <c r="A162">
         <v>0.2</v>
       </c>
-      <c r="B162" s="14">
+      <c r="B162" s="11">
         <v>1E-3</v>
       </c>
       <c r="C162">
@@ -12887,7 +12884,7 @@
       <c r="A163">
         <v>0.3</v>
       </c>
-      <c r="B163" s="14">
+      <c r="B163" s="11">
         <v>1E-3</v>
       </c>
       <c r="C163">
@@ -12920,7 +12917,7 @@
       <c r="A164">
         <v>0.4</v>
       </c>
-      <c r="B164" s="14">
+      <c r="B164" s="11">
         <v>1E-3</v>
       </c>
       <c r="C164">
@@ -12953,7 +12950,7 @@
       <c r="A165">
         <v>0.5</v>
       </c>
-      <c r="B165" s="14">
+      <c r="B165" s="11">
         <v>1E-3</v>
       </c>
       <c r="C165">
@@ -12986,7 +12983,7 @@
       <c r="A166">
         <v>0.6</v>
       </c>
-      <c r="B166" s="14">
+      <c r="B166" s="11">
         <v>1E-3</v>
       </c>
       <c r="C166">
@@ -13019,7 +13016,7 @@
       <c r="A167">
         <v>0.7</v>
       </c>
-      <c r="B167" s="14">
+      <c r="B167" s="11">
         <v>1E-3</v>
       </c>
       <c r="C167">
@@ -13052,7 +13049,7 @@
       <c r="A168">
         <v>0.8</v>
       </c>
-      <c r="B168" s="14">
+      <c r="B168" s="11">
         <v>1E-3</v>
       </c>
       <c r="C168">
@@ -13085,7 +13082,7 @@
       <c r="A169">
         <v>0.9</v>
       </c>
-      <c r="B169" s="14">
+      <c r="B169" s="11">
         <v>1E-3</v>
       </c>
       <c r="C169">
@@ -13118,7 +13115,7 @@
       <c r="A170">
         <v>1</v>
       </c>
-      <c r="B170" s="14">
+      <c r="B170" s="11">
         <v>1E-3</v>
       </c>
       <c r="C170">
@@ -13151,7 +13148,7 @@
       <c r="A171">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B171" s="14">
+      <c r="B171" s="11">
         <v>1E-3</v>
       </c>
       <c r="C171">
@@ -13184,7 +13181,7 @@
       <c r="A172">
         <v>1.2</v>
       </c>
-      <c r="B172" s="14">
+      <c r="B172" s="11">
         <v>1E-3</v>
       </c>
       <c r="C172">
@@ -13217,7 +13214,7 @@
       <c r="A173">
         <v>1.3</v>
       </c>
-      <c r="B173" s="14">
+      <c r="B173" s="11">
         <v>1E-3</v>
       </c>
       <c r="C173">
@@ -13250,7 +13247,7 @@
       <c r="A174">
         <v>1.4</v>
       </c>
-      <c r="B174" s="14">
+      <c r="B174" s="11">
         <v>1E-3</v>
       </c>
       <c r="C174">
@@ -13283,7 +13280,7 @@
       <c r="A175">
         <v>1.5</v>
       </c>
-      <c r="B175" s="14">
+      <c r="B175" s="11">
         <v>1E-3</v>
       </c>
       <c r="C175">
@@ -13316,7 +13313,7 @@
       <c r="A176">
         <v>1.6</v>
       </c>
-      <c r="B176" s="14">
+      <c r="B176" s="11">
         <v>1E-3</v>
       </c>
       <c r="C176">
@@ -13349,7 +13346,7 @@
       <c r="A177">
         <v>1.7</v>
       </c>
-      <c r="B177" s="14">
+      <c r="B177" s="11">
         <v>1E-3</v>
       </c>
       <c r="C177">
@@ -13382,7 +13379,7 @@
       <c r="A178">
         <v>1.8</v>
       </c>
-      <c r="B178" s="14">
+      <c r="B178" s="11">
         <v>1E-3</v>
       </c>
       <c r="C178">
@@ -13415,7 +13412,7 @@
       <c r="A179">
         <v>1.9</v>
       </c>
-      <c r="B179" s="14">
+      <c r="B179" s="11">
         <v>1E-3</v>
       </c>
       <c r="C179">
@@ -13448,7 +13445,7 @@
       <c r="A180">
         <v>2</v>
       </c>
-      <c r="B180" s="14">
+      <c r="B180" s="11">
         <v>1E-3</v>
       </c>
       <c r="C180">
@@ -13481,7 +13478,7 @@
       <c r="A181">
         <v>2.1</v>
       </c>
-      <c r="B181" s="14">
+      <c r="B181" s="11">
         <v>1E-3</v>
       </c>
       <c r="C181">
@@ -13514,7 +13511,7 @@
       <c r="A182">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B182" s="14">
+      <c r="B182" s="11">
         <v>1E-3</v>
       </c>
       <c r="C182">
@@ -13547,7 +13544,7 @@
       <c r="A183">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B183" s="14">
+      <c r="B183" s="11">
         <v>1E-3</v>
       </c>
       <c r="C183">
@@ -13580,7 +13577,7 @@
       <c r="A184">
         <v>2.4</v>
       </c>
-      <c r="B184" s="14">
+      <c r="B184" s="11">
         <v>1E-3</v>
       </c>
       <c r="C184">
@@ -13613,7 +13610,7 @@
       <c r="A185">
         <v>2.5</v>
       </c>
-      <c r="B185" s="14">
+      <c r="B185" s="11">
         <v>1E-3</v>
       </c>
       <c r="C185">
@@ -13646,7 +13643,7 @@
       <c r="A186">
         <v>2.6</v>
       </c>
-      <c r="B186" s="14">
+      <c r="B186" s="11">
         <v>1E-3</v>
       </c>
       <c r="C186">
@@ -13679,7 +13676,7 @@
       <c r="A187">
         <v>2.7</v>
       </c>
-      <c r="B187" s="14">
+      <c r="B187" s="11">
         <v>1E-3</v>
       </c>
       <c r="C187">
@@ -13712,7 +13709,7 @@
       <c r="A188">
         <v>2.8</v>
       </c>
-      <c r="B188" s="14">
+      <c r="B188" s="11">
         <v>1E-3</v>
       </c>
       <c r="C188">
@@ -13745,7 +13742,7 @@
       <c r="A189">
         <v>2.9</v>
       </c>
-      <c r="B189" s="14">
+      <c r="B189" s="11">
         <v>1E-3</v>
       </c>
       <c r="C189">
@@ -13778,7 +13775,7 @@
       <c r="A190">
         <v>3</v>
       </c>
-      <c r="B190" s="14">
+      <c r="B190" s="11">
         <v>1E-3</v>
       </c>
       <c r="C190">
@@ -13811,7 +13808,7 @@
       <c r="A191">
         <v>3.1</v>
       </c>
-      <c r="B191" s="14">
+      <c r="B191" s="11">
         <v>1E-3</v>
       </c>
       <c r="C191">
@@ -13844,7 +13841,7 @@
       <c r="A192">
         <v>3.2</v>
       </c>
-      <c r="B192" s="14">
+      <c r="B192" s="11">
         <v>1E-3</v>
       </c>
       <c r="C192">
@@ -13877,7 +13874,7 @@
       <c r="A193">
         <v>3.3</v>
       </c>
-      <c r="B193" s="14">
+      <c r="B193" s="11">
         <v>1E-3</v>
       </c>
       <c r="C193">
@@ -13910,7 +13907,7 @@
       <c r="A194">
         <v>3.4</v>
       </c>
-      <c r="B194" s="14">
+      <c r="B194" s="11">
         <v>1E-3</v>
       </c>
       <c r="C194">
@@ -13943,7 +13940,7 @@
       <c r="A195">
         <v>3.5</v>
       </c>
-      <c r="B195" s="14">
+      <c r="B195" s="11">
         <v>1E-3</v>
       </c>
       <c r="C195">
@@ -13976,7 +13973,7 @@
       <c r="A196">
         <v>3.6</v>
       </c>
-      <c r="B196" s="14">
+      <c r="B196" s="11">
         <v>1E-3</v>
       </c>
       <c r="C196">
@@ -14009,7 +14006,7 @@
       <c r="A197">
         <v>3.7</v>
       </c>
-      <c r="B197" s="14">
+      <c r="B197" s="11">
         <v>1E-3</v>
       </c>
       <c r="C197">
@@ -14042,7 +14039,7 @@
       <c r="A198">
         <v>3.8</v>
       </c>
-      <c r="B198" s="14">
+      <c r="B198" s="11">
         <v>1E-3</v>
       </c>
       <c r="C198">
@@ -14075,7 +14072,7 @@
       <c r="A199">
         <v>3.9</v>
       </c>
-      <c r="B199" s="14">
+      <c r="B199" s="11">
         <v>1E-3</v>
       </c>
       <c r="C199">
@@ -14108,7 +14105,7 @@
       <c r="A200">
         <v>4</v>
       </c>
-      <c r="B200" s="14">
+      <c r="B200" s="11">
         <v>1E-3</v>
       </c>
       <c r="C200">
@@ -14141,7 +14138,7 @@
       <c r="A201">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B201" s="14">
+      <c r="B201" s="11">
         <v>1E-3</v>
       </c>
       <c r="C201">
@@ -14174,7 +14171,7 @@
       <c r="A202">
         <v>4.2</v>
       </c>
-      <c r="B202" s="14">
+      <c r="B202" s="11">
         <v>1E-3</v>
       </c>
       <c r="C202">
@@ -14207,7 +14204,7 @@
       <c r="A203">
         <v>4.3</v>
       </c>
-      <c r="B203" s="14">
+      <c r="B203" s="11">
         <v>1E-3</v>
       </c>
       <c r="C203">
@@ -14240,7 +14237,7 @@
       <c r="A204">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B204" s="14">
+      <c r="B204" s="11">
         <v>1E-3</v>
       </c>
       <c r="C204">
@@ -14273,7 +14270,7 @@
       <c r="A205">
         <v>4.5</v>
       </c>
-      <c r="B205" s="14">
+      <c r="B205" s="11">
         <v>1E-3</v>
       </c>
       <c r="C205">
@@ -14306,7 +14303,7 @@
       <c r="A206">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B206" s="14">
+      <c r="B206" s="11">
         <v>1E-3</v>
       </c>
       <c r="C206">
@@ -14339,7 +14336,7 @@
       <c r="A207">
         <v>4.7</v>
       </c>
-      <c r="B207" s="14">
+      <c r="B207" s="11">
         <v>1E-3</v>
       </c>
       <c r="C207">
@@ -14372,7 +14369,7 @@
       <c r="A208">
         <v>4.8</v>
       </c>
-      <c r="B208" s="14">
+      <c r="B208" s="11">
         <v>1E-3</v>
       </c>
       <c r="C208">
@@ -14405,7 +14402,7 @@
       <c r="A209">
         <v>4.9000000000000004</v>
       </c>
-      <c r="B209" s="14">
+      <c r="B209" s="11">
         <v>1E-3</v>
       </c>
       <c r="C209">
@@ -14438,7 +14435,7 @@
       <c r="A210">
         <v>5</v>
       </c>
-      <c r="B210" s="14">
+      <c r="B210" s="11">
         <v>1E-3</v>
       </c>
       <c r="C210">
@@ -14471,7 +14468,7 @@
       <c r="A212">
         <v>0.1</v>
       </c>
-      <c r="B212" s="14">
+      <c r="B212" s="11">
         <v>1E-3</v>
       </c>
       <c r="C212">
@@ -14504,7 +14501,7 @@
       <c r="A213">
         <v>0.2</v>
       </c>
-      <c r="B213" s="14">
+      <c r="B213" s="11">
         <v>1E-3</v>
       </c>
       <c r="C213">
@@ -14537,7 +14534,7 @@
       <c r="A214">
         <v>0.3</v>
       </c>
-      <c r="B214" s="14">
+      <c r="B214" s="11">
         <v>1E-3</v>
       </c>
       <c r="C214">
@@ -14570,7 +14567,7 @@
       <c r="A215">
         <v>0.4</v>
       </c>
-      <c r="B215" s="14">
+      <c r="B215" s="11">
         <v>1E-3</v>
       </c>
       <c r="C215">
@@ -14603,7 +14600,7 @@
       <c r="A216">
         <v>0.5</v>
       </c>
-      <c r="B216" s="14">
+      <c r="B216" s="11">
         <v>1E-3</v>
       </c>
       <c r="C216">
@@ -14636,7 +14633,7 @@
       <c r="A217">
         <v>0.6</v>
       </c>
-      <c r="B217" s="14">
+      <c r="B217" s="11">
         <v>1E-3</v>
       </c>
       <c r="C217">
@@ -14669,7 +14666,7 @@
       <c r="A218">
         <v>0.7</v>
       </c>
-      <c r="B218" s="14">
+      <c r="B218" s="11">
         <v>1E-3</v>
       </c>
       <c r="C218">
@@ -14702,7 +14699,7 @@
       <c r="A219">
         <v>0.8</v>
       </c>
-      <c r="B219" s="14">
+      <c r="B219" s="11">
         <v>1E-3</v>
       </c>
       <c r="C219">
@@ -14735,7 +14732,7 @@
       <c r="A220">
         <v>0.9</v>
       </c>
-      <c r="B220" s="14">
+      <c r="B220" s="11">
         <v>1E-3</v>
       </c>
       <c r="C220">
@@ -14768,7 +14765,7 @@
       <c r="A221">
         <v>1</v>
       </c>
-      <c r="B221" s="14">
+      <c r="B221" s="11">
         <v>1E-3</v>
       </c>
       <c r="C221">
@@ -14801,7 +14798,7 @@
       <c r="A222">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B222" s="14">
+      <c r="B222" s="11">
         <v>1E-3</v>
       </c>
       <c r="C222">
@@ -14834,7 +14831,7 @@
       <c r="A223">
         <v>1.2</v>
       </c>
-      <c r="B223" s="14">
+      <c r="B223" s="11">
         <v>1E-3</v>
       </c>
       <c r="C223">
@@ -14867,7 +14864,7 @@
       <c r="A224">
         <v>1.3</v>
       </c>
-      <c r="B224" s="14">
+      <c r="B224" s="11">
         <v>1E-3</v>
       </c>
       <c r="C224">
@@ -14900,7 +14897,7 @@
       <c r="A225">
         <v>1.4</v>
       </c>
-      <c r="B225" s="14">
+      <c r="B225" s="11">
         <v>1E-3</v>
       </c>
       <c r="C225">
@@ -14933,7 +14930,7 @@
       <c r="A226">
         <v>1.5</v>
       </c>
-      <c r="B226" s="14">
+      <c r="B226" s="11">
         <v>1E-3</v>
       </c>
       <c r="C226">
@@ -14966,7 +14963,7 @@
       <c r="A227">
         <v>1.6</v>
       </c>
-      <c r="B227" s="14">
+      <c r="B227" s="11">
         <v>1E-3</v>
       </c>
       <c r="C227">
@@ -14999,7 +14996,7 @@
       <c r="A228">
         <v>1.7</v>
       </c>
-      <c r="B228" s="14">
+      <c r="B228" s="11">
         <v>1E-3</v>
       </c>
       <c r="C228">
@@ -15032,7 +15029,7 @@
       <c r="A229">
         <v>1.8</v>
       </c>
-      <c r="B229" s="14">
+      <c r="B229" s="11">
         <v>1E-3</v>
       </c>
       <c r="C229">
@@ -15065,7 +15062,7 @@
       <c r="A230">
         <v>1.9</v>
       </c>
-      <c r="B230" s="14">
+      <c r="B230" s="11">
         <v>1E-3</v>
       </c>
       <c r="C230">
@@ -15098,7 +15095,7 @@
       <c r="A231">
         <v>2</v>
       </c>
-      <c r="B231" s="14">
+      <c r="B231" s="11">
         <v>1E-3</v>
       </c>
       <c r="C231">
@@ -15131,7 +15128,7 @@
       <c r="A232">
         <v>2.1</v>
       </c>
-      <c r="B232" s="14">
+      <c r="B232" s="11">
         <v>1E-3</v>
       </c>
       <c r="C232">
@@ -15164,7 +15161,7 @@
       <c r="A233">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B233" s="14">
+      <c r="B233" s="11">
         <v>1E-3</v>
       </c>
       <c r="C233">
@@ -15197,7 +15194,7 @@
       <c r="A234">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B234" s="14">
+      <c r="B234" s="11">
         <v>1E-3</v>
       </c>
       <c r="C234">
@@ -15230,7 +15227,7 @@
       <c r="A235">
         <v>2.4</v>
       </c>
-      <c r="B235" s="14">
+      <c r="B235" s="11">
         <v>1E-3</v>
       </c>
       <c r="C235">
@@ -15263,7 +15260,7 @@
       <c r="A236">
         <v>2.5</v>
       </c>
-      <c r="B236" s="14">
+      <c r="B236" s="11">
         <v>1E-3</v>
       </c>
       <c r="C236">
@@ -15296,7 +15293,7 @@
       <c r="A237">
         <v>2.6</v>
       </c>
-      <c r="B237" s="14">
+      <c r="B237" s="11">
         <v>1E-3</v>
       </c>
       <c r="C237">
@@ -15329,7 +15326,7 @@
       <c r="A238">
         <v>2.7</v>
       </c>
-      <c r="B238" s="14">
+      <c r="B238" s="11">
         <v>1E-3</v>
       </c>
       <c r="C238">
@@ -15362,7 +15359,7 @@
       <c r="A239">
         <v>2.8</v>
       </c>
-      <c r="B239" s="14">
+      <c r="B239" s="11">
         <v>1E-3</v>
       </c>
       <c r="C239">
@@ -15395,7 +15392,7 @@
       <c r="A240">
         <v>2.9</v>
       </c>
-      <c r="B240" s="14">
+      <c r="B240" s="11">
         <v>1E-3</v>
       </c>
       <c r="C240">
@@ -15428,7 +15425,7 @@
       <c r="A241">
         <v>3</v>
       </c>
-      <c r="B241" s="14">
+      <c r="B241" s="11">
         <v>1E-3</v>
       </c>
       <c r="C241">
@@ -15461,7 +15458,7 @@
       <c r="A242">
         <v>3.1</v>
       </c>
-      <c r="B242" s="14">
+      <c r="B242" s="11">
         <v>1E-3</v>
       </c>
       <c r="C242">
@@ -15494,7 +15491,7 @@
       <c r="A243">
         <v>3.2</v>
       </c>
-      <c r="B243" s="14">
+      <c r="B243" s="11">
         <v>1E-3</v>
       </c>
       <c r="C243">
@@ -15527,7 +15524,7 @@
       <c r="A244">
         <v>3.3</v>
       </c>
-      <c r="B244" s="14">
+      <c r="B244" s="11">
         <v>1E-3</v>
       </c>
       <c r="C244">
@@ -15560,7 +15557,7 @@
       <c r="A245">
         <v>3.4</v>
       </c>
-      <c r="B245" s="14">
+      <c r="B245" s="11">
         <v>1E-3</v>
       </c>
       <c r="C245">
@@ -15593,7 +15590,7 @@
       <c r="A246">
         <v>3.5</v>
       </c>
-      <c r="B246" s="14">
+      <c r="B246" s="11">
         <v>1E-3</v>
       </c>
       <c r="C246">
@@ -15626,7 +15623,7 @@
       <c r="A247">
         <v>3.6</v>
       </c>
-      <c r="B247" s="14">
+      <c r="B247" s="11">
         <v>1E-3</v>
       </c>
       <c r="C247">
@@ -15659,7 +15656,7 @@
       <c r="A248">
         <v>3.7</v>
       </c>
-      <c r="B248" s="14">
+      <c r="B248" s="11">
         <v>1E-3</v>
       </c>
       <c r="C248">
@@ -15692,7 +15689,7 @@
       <c r="A249">
         <v>3.8</v>
       </c>
-      <c r="B249" s="14">
+      <c r="B249" s="11">
         <v>1E-3</v>
       </c>
       <c r="C249">
@@ -15725,7 +15722,7 @@
       <c r="A250">
         <v>3.9</v>
       </c>
-      <c r="B250" s="14">
+      <c r="B250" s="11">
         <v>1E-3</v>
       </c>
       <c r="C250">
@@ -15758,7 +15755,7 @@
       <c r="A251">
         <v>4</v>
       </c>
-      <c r="B251" s="14">
+      <c r="B251" s="11">
         <v>1E-3</v>
       </c>
       <c r="C251">
@@ -15791,7 +15788,7 @@
       <c r="A252">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B252" s="14">
+      <c r="B252" s="11">
         <v>1E-3</v>
       </c>
       <c r="C252">
@@ -15824,7 +15821,7 @@
       <c r="A253">
         <v>4.2</v>
       </c>
-      <c r="B253" s="14">
+      <c r="B253" s="11">
         <v>1E-3</v>
       </c>
       <c r="C253">
@@ -15857,7 +15854,7 @@
       <c r="A254">
         <v>4.3</v>
       </c>
-      <c r="B254" s="14">
+      <c r="B254" s="11">
         <v>1E-3</v>
       </c>
       <c r="C254">
@@ -15890,7 +15887,7 @@
       <c r="A255">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B255" s="14">
+      <c r="B255" s="11">
         <v>1E-3</v>
       </c>
       <c r="C255">
@@ -15923,7 +15920,7 @@
       <c r="A256">
         <v>4.5</v>
       </c>
-      <c r="B256" s="14">
+      <c r="B256" s="11">
         <v>1E-3</v>
       </c>
       <c r="C256">
@@ -15956,7 +15953,7 @@
       <c r="A257">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B257" s="14">
+      <c r="B257" s="11">
         <v>1E-3</v>
       </c>
       <c r="C257">
@@ -15989,7 +15986,7 @@
       <c r="A258">
         <v>4.7</v>
       </c>
-      <c r="B258" s="14">
+      <c r="B258" s="11">
         <v>1E-3</v>
       </c>
       <c r="C258">
@@ -16022,7 +16019,7 @@
       <c r="A259">
         <v>4.8</v>
       </c>
-      <c r="B259" s="14">
+      <c r="B259" s="11">
         <v>1E-3</v>
       </c>
       <c r="C259">
@@ -16055,7 +16052,7 @@
       <c r="A260">
         <v>4.9000000000000004</v>
       </c>
-      <c r="B260" s="14">
+      <c r="B260" s="11">
         <v>1E-3</v>
       </c>
       <c r="C260">
@@ -16088,7 +16085,7 @@
       <c r="A261">
         <v>5</v>
       </c>
-      <c r="B261" s="14">
+      <c r="B261" s="11">
         <v>1E-3</v>
       </c>
       <c r="C261">
@@ -16164,10 +16161,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="T167" sqref="T167"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16292,7 +16289,7 @@
       <c r="A8">
         <v>0.5</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="11">
         <v>1E-3</v>
       </c>
       <c r="C8">
@@ -16320,7 +16317,7 @@
         <v>49.653086777802301</v>
       </c>
       <c r="K8">
-        <f t="shared" ref="K8:K18" si="0">AVERAGE(E8:J8)</f>
+        <f t="shared" ref="K8:K16" si="0">AVERAGE(E8:J8)</f>
         <v>59.363265210059801</v>
       </c>
     </row>
@@ -16328,7 +16325,7 @@
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="11">
         <v>1E-3</v>
       </c>
       <c r="C9">
@@ -16364,7 +16361,7 @@
       <c r="A10">
         <v>1.5</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="11">
         <v>1E-3</v>
       </c>
       <c r="C10">
@@ -16400,7 +16397,7 @@
       <c r="A11">
         <v>2</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="11">
         <v>1E-3</v>
       </c>
       <c r="C11">
@@ -16436,7 +16433,7 @@
       <c r="A12">
         <v>2.5</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="11">
         <v>1E-3</v>
       </c>
       <c r="C12">
@@ -16472,7 +16469,7 @@
       <c r="A13">
         <v>3</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="11">
         <v>1E-3</v>
       </c>
       <c r="C13">
@@ -16508,7 +16505,7 @@
       <c r="A14">
         <v>3.5</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="11">
         <v>1E-3</v>
       </c>
       <c r="C14">
@@ -16544,7 +16541,7 @@
       <c r="A15">
         <v>4</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="11">
         <v>1E-3</v>
       </c>
       <c r="C15">
@@ -16580,7 +16577,7 @@
       <c r="A16">
         <v>4.5</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="11">
         <v>1E-3</v>
       </c>
       <c r="C16">
@@ -16612,720 +16609,822 @@
         <v>22.578958662582767</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>5</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="11">
         <v>1E-3</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>0.5</v>
-      </c>
-      <c r="B19">
+        <v>0.1</v>
+      </c>
+      <c r="B19" s="11">
         <v>0.01</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="D19">
-        <v>50637</v>
-      </c>
       <c r="E19">
-        <v>66.0291806140782</v>
+        <v>71.790000000000006</v>
       </c>
       <c r="F19">
-        <v>65.574633402860002</v>
+        <v>63.4</v>
       </c>
       <c r="G19">
-        <v>67.728129296707706</v>
+        <v>69.998999999999995</v>
       </c>
       <c r="H19">
-        <v>54.289840684406698</v>
+        <v>56.899000000000001</v>
       </c>
       <c r="I19">
-        <v>53.176073763646201</v>
+        <v>53.04</v>
       </c>
       <c r="J19">
-        <v>50.109007897479799</v>
+        <v>42.37</v>
       </c>
       <c r="K19">
-        <f t="shared" ref="K19:K26" si="1">AVERAGE(E19:J19)</f>
-        <v>59.484477609863099</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+        <f>AVERAGE(E19:J19)</f>
+        <v>59.582999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20">
+        <v>0.25</v>
+      </c>
+      <c r="B20" s="11">
         <v>0.01</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20">
+        <v>67673</v>
+      </c>
+      <c r="E20">
+        <v>70.260000000000005</v>
+      </c>
+      <c r="F20">
+        <v>64.34</v>
+      </c>
+      <c r="G20">
+        <v>68.98</v>
+      </c>
+      <c r="H20">
+        <v>56.11</v>
+      </c>
+      <c r="I20">
+        <v>53.47</v>
+      </c>
+      <c r="J20">
+        <v>45.19</v>
+      </c>
+      <c r="K20">
+        <f>AVERAGE(E20:J20)</f>
+        <v>59.725000000000016</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0.5</v>
+      </c>
+      <c r="B21">
+        <v>0.01</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>50637</v>
+      </c>
+      <c r="E21">
+        <v>66.0291806140782</v>
+      </c>
+      <c r="F21">
+        <v>65.574633402860002</v>
+      </c>
+      <c r="G21">
+        <v>67.728129296707706</v>
+      </c>
+      <c r="H21">
+        <v>54.289840684406698</v>
+      </c>
+      <c r="I21">
+        <v>53.176073763646201</v>
+      </c>
+      <c r="J21">
+        <v>50.109007897479799</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ref="K21:K28" si="1">AVERAGE(E21:J21)</f>
+        <v>59.484477609863099</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>0.01</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
         <v>50760</v>
       </c>
-      <c r="E20">
+      <c r="E22">
         <v>54.254612225415698</v>
       </c>
-      <c r="F20">
+      <c r="F22">
         <v>62.890653906083102</v>
       </c>
-      <c r="G20">
+      <c r="G22">
         <v>61.641662623269198</v>
       </c>
-      <c r="H20">
+      <c r="H22">
         <v>48.672154256651098</v>
       </c>
-      <c r="I20">
+      <c r="I22">
         <v>48.920417228377602</v>
       </c>
-      <c r="J20">
+      <c r="J22">
         <v>55.427965866655398</v>
       </c>
-      <c r="K20">
+      <c r="K22">
         <f t="shared" si="1"/>
         <v>55.301244351075354</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>1.5</v>
       </c>
-      <c r="B21">
-        <v>0.01</v>
-      </c>
-      <c r="C21">
+      <c r="B23">
+        <v>0.01</v>
+      </c>
+      <c r="C23">
         <v>1</v>
       </c>
-      <c r="D21">
+      <c r="D23">
         <v>121634</v>
       </c>
-      <c r="E21">
+      <c r="E23">
         <v>27.996385518194401</v>
       </c>
-      <c r="F21">
+      <c r="F23">
         <v>41.066649360351299</v>
       </c>
-      <c r="G21">
+      <c r="G23">
         <v>35.600018892258099</v>
       </c>
-      <c r="H21">
+      <c r="H23">
         <v>26.492268993609699</v>
       </c>
-      <c r="I21">
+      <c r="I23">
         <v>30.223944361576802</v>
       </c>
-      <c r="J21">
+      <c r="J23">
         <v>44.270940797026597</v>
       </c>
-      <c r="K21">
+      <c r="K23">
         <f t="shared" si="1"/>
         <v>34.275034653836144</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="B22">
-        <v>0.01</v>
-      </c>
-      <c r="C22">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>0.01</v>
+      </c>
+      <c r="C24">
         <v>1</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>113825</v>
       </c>
-      <c r="E22">
+      <c r="E24">
         <v>12.7773713169288</v>
       </c>
-      <c r="F22">
+      <c r="F24">
         <v>28.521766878598399</v>
       </c>
-      <c r="G22">
+      <c r="G24">
         <v>24.430247880996099</v>
       </c>
-      <c r="H22">
+      <c r="H24">
         <v>16.268212150236501</v>
       </c>
-      <c r="I22">
+      <c r="I24">
         <v>18.9208325831218</v>
       </c>
-      <c r="J22">
+      <c r="J24">
         <v>37.755651518395197</v>
       </c>
-      <c r="K22">
+      <c r="K24">
         <f t="shared" si="1"/>
         <v>23.112347054712803</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>2.5</v>
       </c>
-      <c r="B23">
-        <v>0.01</v>
-      </c>
-      <c r="C23">
+      <c r="B25">
+        <v>0.01</v>
+      </c>
+      <c r="C25">
         <v>1</v>
       </c>
-      <c r="D23">
+      <c r="D25">
         <v>266226</v>
       </c>
-      <c r="E23">
+      <c r="E25">
         <v>9.4197729000916404</v>
       </c>
-      <c r="F23">
+      <c r="F25">
         <v>24.451592329047202</v>
       </c>
-      <c r="G23">
+      <c r="G25">
         <v>21.498655473282401</v>
       </c>
-      <c r="H23">
+      <c r="H25">
         <v>11.5961447242923</v>
       </c>
-      <c r="I23">
+      <c r="I25">
         <v>12.401853572978499</v>
       </c>
-      <c r="J23">
+      <c r="J25">
         <v>33.593692545978399</v>
       </c>
-      <c r="K23">
+      <c r="K25">
         <f t="shared" si="1"/>
         <v>18.826951924278408</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>3</v>
       </c>
-      <c r="B24">
-        <v>0.01</v>
-      </c>
-      <c r="C24">
+      <c r="B26">
+        <v>0.01</v>
+      </c>
+      <c r="C26">
         <v>1</v>
       </c>
-      <c r="D24">
+      <c r="D26">
         <v>339376</v>
       </c>
-      <c r="E24">
+      <c r="E26">
         <v>9.3546753512747198</v>
       </c>
-      <c r="F24">
+      <c r="F26">
         <v>21.315518264288102</v>
       </c>
-      <c r="G24">
+      <c r="G26">
         <v>20.316844315652101</v>
       </c>
-      <c r="H24">
+      <c r="H26">
         <v>10.0518383383095</v>
       </c>
-      <c r="I24">
+      <c r="I26">
         <v>7.8091196488574202</v>
       </c>
-      <c r="J24">
+      <c r="J26">
         <v>30.239982559904799</v>
       </c>
-      <c r="K24">
+      <c r="K26">
         <f t="shared" si="1"/>
         <v>16.514663079714442</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>3.5</v>
       </c>
-      <c r="B25">
-        <v>0.01</v>
-      </c>
-      <c r="C25">
+      <c r="B27">
+        <v>0.01</v>
+      </c>
+      <c r="C27">
         <v>1</v>
       </c>
-      <c r="D25">
+      <c r="D27">
         <v>339376</v>
       </c>
-      <c r="E25">
+      <c r="E27">
         <v>11.4580930253577</v>
       </c>
-      <c r="F25">
+      <c r="F27">
         <v>19.4156742084126</v>
       </c>
-      <c r="G25">
+      <c r="G27">
         <v>20.392206462463498</v>
       </c>
-      <c r="H25">
+      <c r="H27">
         <v>10.390438493313701</v>
       </c>
-      <c r="I25">
+      <c r="I27">
         <v>4.7095736492276998</v>
       </c>
-      <c r="J25">
+      <c r="J27">
         <v>27.7715523083458</v>
       </c>
-      <c r="K25">
+      <c r="K27">
         <f t="shared" si="1"/>
         <v>15.689589691186834</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28">
         <v>4</v>
       </c>
-      <c r="B26">
-        <v>0.01</v>
-      </c>
-      <c r="C26">
+      <c r="B28">
+        <v>0.01</v>
+      </c>
+      <c r="C28">
         <v>1</v>
       </c>
-      <c r="E26">
+      <c r="E28">
         <v>14.004691991519801</v>
       </c>
-      <c r="F26">
+      <c r="F28">
         <v>18.102928855766301</v>
       </c>
-      <c r="G26">
+      <c r="G28">
         <v>20.7907240768936</v>
       </c>
-      <c r="H26">
+      <c r="H28">
         <v>11.5411421705577</v>
       </c>
-      <c r="I26">
+      <c r="I28">
         <v>2.9647181816144599</v>
       </c>
-      <c r="J26">
+      <c r="J28">
         <v>25.7290589370083</v>
       </c>
-      <c r="K26">
+      <c r="K28">
         <f t="shared" si="1"/>
         <v>15.522210702226694</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29">
         <v>4.5</v>
       </c>
-      <c r="B27">
-        <v>0.01</v>
-      </c>
-      <c r="C27">
+      <c r="B29">
+        <v>0.01</v>
+      </c>
+      <c r="C29">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30">
         <v>5</v>
       </c>
-      <c r="B28">
-        <v>0.01</v>
-      </c>
-      <c r="C28">
+      <c r="B30">
+        <v>0.01</v>
+      </c>
+      <c r="C30">
         <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>0.5</v>
-      </c>
-      <c r="B31">
-        <v>0.01</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31">
-        <v>50878</v>
-      </c>
-      <c r="E31">
-        <v>66.550560709649304</v>
-      </c>
-      <c r="F31">
-        <v>65.455267811711394</v>
-      </c>
-      <c r="G31">
-        <v>67.356542275890206</v>
-      </c>
-      <c r="H31">
-        <v>54.3256288046897</v>
-      </c>
-      <c r="I31">
-        <v>53.392320439518201</v>
-      </c>
-      <c r="J31">
-        <v>49.494643993594103</v>
-      </c>
-      <c r="K31">
-        <f>AVERAGE(E31:J31)</f>
-        <v>59.429160672508807</v>
-      </c>
-      <c r="L31">
-        <f>AVERAGE(E31:I31)</f>
-        <v>61.416064008291755</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>1</v>
-      </c>
-      <c r="B32">
-        <v>0.01</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
-      <c r="D32">
-        <v>51549</v>
-      </c>
-      <c r="E32">
-        <v>55.107499544095297</v>
-      </c>
-      <c r="F32">
-        <v>63.438779145715301</v>
-      </c>
-      <c r="G32">
-        <v>62.2942381849996</v>
-      </c>
-      <c r="H32">
-        <v>49.378102440029302</v>
-      </c>
-      <c r="I32">
-        <v>49.386820220588497</v>
-      </c>
-      <c r="J32">
-        <v>55.5470499054939</v>
-      </c>
-      <c r="K32">
-        <f t="shared" ref="K32:K40" si="2">AVERAGE(E32:J32)</f>
-        <v>55.858748240153652</v>
-      </c>
-      <c r="L32">
-        <f t="shared" ref="L32:L40" si="3">AVERAGE(E32:I32)</f>
-        <v>55.9210879070856</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
+        <v>0.25</v>
+      </c>
+      <c r="B33">
+        <v>0.01</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>70.48</v>
+      </c>
+      <c r="F33">
+        <v>63.75</v>
+      </c>
+      <c r="G33">
+        <v>68.63</v>
+      </c>
+      <c r="H33">
+        <v>56.07</v>
+      </c>
+      <c r="I33">
+        <v>53.38</v>
+      </c>
+      <c r="J33">
+        <v>44.47</v>
+      </c>
+      <c r="K33">
+        <f>AVERAGE(E33:J33)</f>
+        <v>59.463333333333331</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0.5</v>
+      </c>
+      <c r="B34">
+        <v>0.01</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>50878</v>
+      </c>
+      <c r="E34">
+        <v>66.550560709649304</v>
+      </c>
+      <c r="F34">
+        <v>65.455267811711394</v>
+      </c>
+      <c r="G34">
+        <v>67.356542275890206</v>
+      </c>
+      <c r="H34">
+        <v>54.3256288046897</v>
+      </c>
+      <c r="I34">
+        <v>53.392320439518201</v>
+      </c>
+      <c r="J34">
+        <v>49.494643993594103</v>
+      </c>
+      <c r="K34">
+        <f>AVERAGE(E34:J34)</f>
+        <v>59.429160672508807</v>
+      </c>
+      <c r="L34">
+        <f>AVERAGE(E34:I34)</f>
+        <v>61.416064008291755</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>0.01</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>51549</v>
+      </c>
+      <c r="E35">
+        <v>55.107499544095297</v>
+      </c>
+      <c r="F35">
+        <v>63.438779145715301</v>
+      </c>
+      <c r="G35">
+        <v>62.2942381849996</v>
+      </c>
+      <c r="H35">
+        <v>49.378102440029302</v>
+      </c>
+      <c r="I35">
+        <v>49.386820220588497</v>
+      </c>
+      <c r="J35">
+        <v>55.5470499054939</v>
+      </c>
+      <c r="K35">
+        <f t="shared" ref="K35:K43" si="2">AVERAGE(E35:J35)</f>
+        <v>55.858748240153652</v>
+      </c>
+      <c r="L35">
+        <f t="shared" ref="L35:L43" si="3">AVERAGE(E35:I35)</f>
+        <v>55.9210879070856</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36">
         <v>1.5</v>
       </c>
-      <c r="B33">
-        <v>0.01</v>
-      </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-      <c r="D33">
+      <c r="B36">
+        <v>0.01</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
         <v>71920</v>
       </c>
-      <c r="E33">
+      <c r="E36">
         <v>30.222889949716102</v>
       </c>
-      <c r="F33">
+      <c r="F36">
         <v>43.723866181811097</v>
       </c>
-      <c r="G33">
+      <c r="G36">
         <v>38.938018063285803</v>
       </c>
-      <c r="H33">
+      <c r="H36">
         <v>29.638977395260799</v>
       </c>
-      <c r="I33">
+      <c r="I36">
         <v>32.421503195158003</v>
       </c>
-      <c r="J33">
+      <c r="J36">
         <v>46.486163379173</v>
       </c>
-      <c r="K33">
+      <c r="K36">
         <f t="shared" si="2"/>
         <v>36.905236360734136</v>
       </c>
-      <c r="L33">
+      <c r="L36">
         <f t="shared" si="3"/>
         <v>34.989050957046359</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>2</v>
-      </c>
-      <c r="B34">
-        <v>0.01</v>
-      </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
-      <c r="D34">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37">
+        <v>0.01</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
         <v>75865</v>
       </c>
-      <c r="E34">
+      <c r="E37">
         <v>18.616907171074299</v>
       </c>
-      <c r="F34">
+      <c r="F37">
         <v>34.019742234961797</v>
       </c>
-      <c r="G34">
+      <c r="G37">
         <v>30.298106784971001</v>
       </c>
-      <c r="H34">
+      <c r="H37">
         <v>21.037285202150301</v>
       </c>
-      <c r="I34">
+      <c r="I37">
         <v>22.2704847692426</v>
       </c>
-      <c r="J34">
+      <c r="J37">
         <v>40.825283792361503</v>
       </c>
-      <c r="K34">
+      <c r="K37">
         <f t="shared" si="2"/>
         <v>27.844634992460254</v>
       </c>
-      <c r="L34">
+      <c r="L37">
         <f t="shared" si="3"/>
         <v>25.248505232479999</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38">
         <v>2.5</v>
       </c>
-      <c r="B35">
-        <v>0.01</v>
-      </c>
-      <c r="C35">
-        <v>2</v>
-      </c>
-      <c r="D35">
+      <c r="B38">
+        <v>0.01</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
         <v>88033</v>
       </c>
-      <c r="E35">
+      <c r="E38">
         <v>16.7734742838622</v>
       </c>
-      <c r="F35">
+      <c r="F38">
         <v>31.303114519484598</v>
       </c>
-      <c r="G35">
+      <c r="G38">
         <v>28.925684850707601</v>
       </c>
-      <c r="H35">
+      <c r="H38">
         <v>18.122028644137298</v>
       </c>
-      <c r="I35">
+      <c r="I38">
         <v>17.0356546094471</v>
       </c>
-      <c r="J35">
+      <c r="J38">
         <v>36.752516862849703</v>
       </c>
-      <c r="K35">
+      <c r="K38">
         <f t="shared" si="2"/>
         <v>24.818745628414746</v>
       </c>
-      <c r="L35">
+      <c r="L38">
         <f t="shared" si="3"/>
         <v>22.431991381527759</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39">
         <v>3</v>
       </c>
-      <c r="B36">
-        <v>0.01</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-      <c r="D36">
+      <c r="B39">
+        <v>0.01</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
         <v>119015</v>
       </c>
-      <c r="E36">
+      <c r="E39">
         <v>16.995628100860198</v>
       </c>
-      <c r="F36">
+      <c r="F39">
         <v>29.782132239153</v>
       </c>
-      <c r="G36">
+      <c r="G39">
         <v>28.8543949342329</v>
       </c>
-      <c r="H36">
+      <c r="H39">
         <v>17.445561296022699</v>
       </c>
-      <c r="I36">
+      <c r="I39">
         <v>13.956936684577601</v>
       </c>
-      <c r="J36">
+      <c r="J39">
         <v>33.7550464748075</v>
       </c>
-      <c r="K36">
+      <c r="K39">
         <f t="shared" si="2"/>
         <v>23.464949954942316</v>
       </c>
-      <c r="L36">
+      <c r="L39">
         <f t="shared" si="3"/>
         <v>21.406930650969279</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40">
         <v>3.5</v>
       </c>
-      <c r="B37">
-        <v>0.01</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37">
+      <c r="B40">
+        <v>0.01</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
         <v>128356</v>
       </c>
-      <c r="E37">
+      <c r="E40">
         <v>18.263677513309901</v>
       </c>
-      <c r="F37">
+      <c r="F40">
         <v>28.782429827186899</v>
       </c>
-      <c r="G37">
+      <c r="G40">
         <v>29.4389110466308</v>
       </c>
-      <c r="H37">
+      <c r="H40">
         <v>17.572236315801799</v>
       </c>
-      <c r="I37">
+      <c r="I40">
         <v>11.9789337564831</v>
       </c>
-      <c r="J37">
+      <c r="J40">
         <v>31.552625310596898</v>
       </c>
-      <c r="K37">
+      <c r="K40">
         <f t="shared" si="2"/>
         <v>22.931468961668234</v>
       </c>
-      <c r="L37">
+      <c r="L40">
         <f t="shared" si="3"/>
         <v>21.207237691882504</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41">
         <v>4</v>
       </c>
-      <c r="B38">
-        <v>0.01</v>
-      </c>
-      <c r="C38">
-        <v>2</v>
-      </c>
-      <c r="D38">
+      <c r="B41">
+        <v>0.01</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
         <v>167513</v>
       </c>
-      <c r="E38">
+      <c r="E41">
         <v>20.187867132748799</v>
       </c>
-      <c r="F38">
+      <c r="F41">
         <v>28.4163407721223</v>
       </c>
-      <c r="G38">
+      <c r="G41">
         <v>30.257801305936098</v>
       </c>
-      <c r="H38">
+      <c r="H41">
         <v>18.646935314348099</v>
       </c>
-      <c r="I38">
+      <c r="I41">
         <v>11.1981613080734</v>
       </c>
-      <c r="J38">
+      <c r="J41">
         <v>29.758992189607099</v>
       </c>
-      <c r="K38">
+      <c r="K41">
         <f t="shared" si="2"/>
         <v>23.077683003805969</v>
       </c>
-      <c r="L38">
+      <c r="L41">
         <f t="shared" si="3"/>
         <v>21.74142116664574</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42">
         <v>4.5</v>
       </c>
-      <c r="B39">
-        <v>0.01</v>
-      </c>
-      <c r="C39">
-        <v>2</v>
-      </c>
-      <c r="D39">
+      <c r="B42">
+        <v>0.01</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
         <v>192369</v>
       </c>
-      <c r="E39">
+      <c r="E42">
         <v>22.003691854420001</v>
       </c>
-      <c r="F39">
+      <c r="F42">
         <v>28.331500649080699</v>
       </c>
-      <c r="G39">
+      <c r="G42">
         <v>31.1157701996692</v>
       </c>
-      <c r="H39">
+      <c r="H42">
         <v>19.606209358592501</v>
       </c>
-      <c r="I39">
+      <c r="I42">
         <v>10.917595218970201</v>
       </c>
-      <c r="J39">
+      <c r="J42">
         <v>28.292931151129899</v>
       </c>
-      <c r="K39">
+      <c r="K42">
         <f t="shared" si="2"/>
         <v>23.37794973864375</v>
       </c>
-      <c r="L39">
+      <c r="L42">
         <f t="shared" si="3"/>
         <v>22.394953456146521</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43">
         <v>5</v>
       </c>
-      <c r="B40">
-        <v>0.01</v>
-      </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-      <c r="D40">
+      <c r="B43">
+        <v>0.01</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
         <v>249395</v>
       </c>
-      <c r="E40">
+      <c r="E43">
         <v>23.636593418985999</v>
       </c>
-      <c r="F40">
+      <c r="F43">
         <v>28.3283159401905</v>
       </c>
-      <c r="G40">
+      <c r="G43">
         <v>31.954415061242599</v>
       </c>
-      <c r="H40">
+      <c r="H43">
         <v>20.635306729882799</v>
       </c>
-      <c r="I40">
+      <c r="I43">
         <v>11.0240011361541</v>
       </c>
-      <c r="J40">
+      <c r="J43">
         <v>27.032575594769501</v>
       </c>
-      <c r="K40">
+      <c r="K43">
         <f t="shared" si="2"/>
         <v>23.768534646870918</v>
       </c>
-      <c r="L40">
+      <c r="L43">
         <f t="shared" si="3"/>
         <v>23.115726457291199</v>
       </c>
@@ -17414,16 +17513,16 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="11">
+      <c r="A3" s="12">
         <v>3</v>
       </c>
-      <c r="B3" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="C3" s="11">
-        <v>2</v>
-      </c>
-      <c r="D3" s="11">
+      <c r="B3" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="C3" s="12">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12">
         <v>90</v>
       </c>
       <c r="E3" s="4">
@@ -17432,150 +17531,150 @@
       <c r="F3" s="4">
         <v>13.1</v>
       </c>
-      <c r="I3" s="13"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="4">
         <v>12.1655</v>
       </c>
       <c r="F4" s="4">
         <v>23.7</v>
       </c>
-      <c r="I4" s="13"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="4">
         <v>16.717199999999998</v>
       </c>
       <c r="F5" s="4">
         <v>22.3</v>
       </c>
-      <c r="I5" s="13"/>
+      <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="4">
         <v>7.9989999999999997</v>
       </c>
       <c r="F6" s="4">
         <v>18.399999999999999</v>
       </c>
-      <c r="I6" s="13"/>
+      <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="4">
         <v>11.8887</v>
       </c>
       <c r="F7" s="4">
         <v>24.7</v>
       </c>
-      <c r="I7" s="13"/>
+      <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
       <c r="E8" s="4">
         <v>13.822900000000001</v>
       </c>
       <c r="F8" s="4">
         <v>26.2</v>
       </c>
-      <c r="I8" s="13"/>
+      <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="4">
         <v>15.4764</v>
       </c>
       <c r="F9" s="4">
         <v>51.3</v>
       </c>
-      <c r="I9" s="13"/>
+      <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="4">
         <v>20.939699999999998</v>
       </c>
       <c r="F10" s="4">
         <v>10.1</v>
       </c>
-      <c r="I10" s="13"/>
+      <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="4">
         <v>18.8032</v>
       </c>
       <c r="F11" s="4">
         <v>12.6</v>
       </c>
-      <c r="I11" s="13"/>
+      <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
       <c r="E12" s="4">
         <v>11.1068</v>
       </c>
       <c r="F12" s="4">
         <v>21.5</v>
       </c>
-      <c r="I12" s="13"/>
+      <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="4">
         <v>1.6796</v>
       </c>
       <c r="F13" s="4">
         <v>26.6</v>
       </c>
-      <c r="I13" s="13"/>
+      <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
       <c r="E14" s="4">
         <v>14.2706</v>
       </c>
       <c r="F14" s="4">
         <v>26.2</v>
       </c>
-      <c r="I14" s="13"/>
+      <c r="I14" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>